<commit_message>
Forgot to add Twitter Dashboard to the excel file
</commit_message>
<xml_diff>
--- a/NiFi Templates.xlsx
+++ b/NiFi Templates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="20" windowWidth="18300" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18420" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="177">
   <si>
     <t>Template Name:</t>
   </si>
@@ -595,6 +595,12 @@
   </si>
   <si>
     <t>An Ad Hoc web service that "enriches" a request to port 8011 with a NiFi greeting utilizing HandleHttpRequest, HandleHttpResponse and the StandardHttpContextMap controller service.</t>
+  </si>
+  <si>
+    <t>Twitter_Dashboard</t>
+  </si>
+  <si>
+    <t>Push tweets to HDFS/Solr and visualize using Banana dashboard.</t>
   </si>
 </sst>
 </file>
@@ -1361,10 +1367,10 @@
   <dimension ref="A1:DR164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="CN33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="CQ34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="CS34" sqref="CS34"/>
+      <selection pane="bottomRight" activeCell="DA34" sqref="DA34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1488,7 +1494,7 @@
       </c>
       <c r="AE1">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AF1">
         <f t="shared" si="1"/>
@@ -1616,7 +1622,7 @@
       </c>
       <c r="BK1">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BL1">
         <f t="shared" si="1"/>
@@ -1672,7 +1678,7 @@
       </c>
       <c r="BY1">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BZ1">
         <f t="shared" si="1"/>
@@ -1704,7 +1710,7 @@
       </c>
       <c r="CG1">
         <f t="shared" ref="CG1:DQ1" si="2">COUNTIFS(CG10:CG300,"X")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="CH1">
         <f t="shared" si="2"/>
@@ -1720,7 +1726,7 @@
       </c>
       <c r="CK1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="CL1">
         <f t="shared" si="2"/>
@@ -1748,7 +1754,7 @@
       </c>
       <c r="CR1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CS1">
         <f t="shared" si="2"/>
@@ -1764,7 +1770,7 @@
       </c>
       <c r="CV1">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="CW1">
         <f t="shared" si="2"/>
@@ -1780,7 +1786,7 @@
       </c>
       <c r="CZ1">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="DA1">
         <f t="shared" si="2"/>
@@ -6131,8 +6137,12 @@
       <c r="DQ33" s="13"/>
     </row>
     <row r="34" spans="1:121" ht="72" customHeight="1">
-      <c r="A34" s="16"/>
-      <c r="B34" s="24"/>
+      <c r="A34" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="B34" s="24" t="s">
+        <v>176</v>
+      </c>
       <c r="D34" s="18"/>
       <c r="E34" s="18"/>
       <c r="F34" s="13"/>
@@ -6160,7 +6170,9 @@
       <c r="AB34" s="13"/>
       <c r="AC34" s="13"/>
       <c r="AD34" s="13"/>
-      <c r="AE34" s="13"/>
+      <c r="AE34" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="AF34" s="13"/>
       <c r="AG34" s="13"/>
       <c r="AH34" s="13"/>
@@ -6192,7 +6204,9 @@
       <c r="BH34" s="13"/>
       <c r="BI34" s="13"/>
       <c r="BJ34" s="13"/>
-      <c r="BK34" s="13"/>
+      <c r="BK34" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="BL34" s="13"/>
       <c r="BM34" s="13"/>
       <c r="BN34" s="13"/>
@@ -6206,7 +6220,9 @@
       <c r="BV34" s="13"/>
       <c r="BW34" s="13"/>
       <c r="BX34" s="13"/>
-      <c r="BY34" s="13"/>
+      <c r="BY34" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="BZ34" s="13"/>
       <c r="CA34" s="13"/>
       <c r="CB34" s="13"/>
@@ -6214,26 +6230,36 @@
       <c r="CD34" s="13"/>
       <c r="CE34" s="13"/>
       <c r="CF34" s="13"/>
-      <c r="CG34" s="13"/>
+      <c r="CG34" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="CH34" s="13"/>
       <c r="CI34" s="13"/>
       <c r="CJ34" s="13"/>
-      <c r="CK34" s="13"/>
+      <c r="CK34" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="CL34" s="13"/>
       <c r="CM34" s="13"/>
       <c r="CN34" s="13"/>
       <c r="CO34" s="13"/>
       <c r="CP34" s="13"/>
       <c r="CQ34" s="13"/>
-      <c r="CR34" s="13"/>
+      <c r="CR34" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="CS34" s="13"/>
       <c r="CT34" s="13"/>
       <c r="CU34" s="13"/>
-      <c r="CV34" s="13"/>
+      <c r="CV34" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="CW34" s="13"/>
       <c r="CX34" s="13"/>
       <c r="CY34" s="13"/>
-      <c r="CZ34" s="13"/>
+      <c r="CZ34" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="DA34" s="13"/>
       <c r="DB34" s="13"/>
       <c r="DC34" s="13"/>

</xml_diff>

<commit_message>
Updating excel file and WebCrawler
</commit_message>
<xml_diff>
--- a/NiFi Templates.xlsx
+++ b/NiFi Templates.xlsx
@@ -607,7 +607,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -659,6 +659,14 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -790,7 +798,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -871,6 +879,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="33">
@@ -954,7 +964,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="83">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1035,6 +1045,8 @@
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1367,10 +1379,10 @@
   <dimension ref="A1:DR164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="CQ34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="D30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="DA34" sqref="DA34"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Adding the PostHTTP_Content-Type template that demonstrates how to specify a Post Http content type
</commit_message>
<xml_diff>
--- a/NiFi Templates.xlsx
+++ b/NiFi Templates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="100" windowWidth="18420" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="18420" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="181">
   <si>
     <t>Template Name:</t>
   </si>
@@ -607,6 +607,12 @@
   </si>
   <si>
     <t>This template is an example of how ListSFTP and FetchSFTP work together to create a list of files on a remote system and then decide which files the user wants to pull from the remote system.</t>
+  </si>
+  <si>
+    <t>PostHTTP Content-Type</t>
+  </si>
+  <si>
+    <t>Sample flow to specify a PostHTTP Content-Type by updating the mime.type on a FlowFile.  These flowfile requests are received by a HandleHttpResponse and a logging of the associated attributes is performed to view how an endpoint would receive the specified headers and content.</t>
   </si>
 </sst>
 </file>
@@ -1385,10 +1391,10 @@
   <dimension ref="A1:DR164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="D35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="DE36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B36" sqref="B36"/>
+      <selection pane="bottomRight" activeCell="DO36" sqref="DO36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1436,7 +1442,7 @@
       </c>
       <c r="K1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L1">
         <f t="shared" si="0"/>
@@ -1580,7 +1586,7 @@
       </c>
       <c r="AV1">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AW1">
         <f t="shared" si="1"/>
@@ -1644,11 +1650,11 @@
       </c>
       <c r="BL1">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BM1">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BN1">
         <f t="shared" si="1"/>
@@ -1692,7 +1698,7 @@
       </c>
       <c r="BX1">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BY1">
         <f t="shared" si="1"/>
@@ -1708,7 +1714,7 @@
       </c>
       <c r="CB1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="CC1">
         <f t="shared" si="1"/>
@@ -1788,7 +1794,7 @@
       </c>
       <c r="CV1">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="CW1">
         <f t="shared" si="2"/>
@@ -1864,7 +1870,7 @@
       </c>
       <c r="DO1">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="DP1">
         <f t="shared" si="2"/>
@@ -6453,8 +6459,12 @@
       <c r="DQ35" s="13"/>
     </row>
     <row r="36" spans="1:121" ht="72" customHeight="1">
-      <c r="A36" s="16"/>
-      <c r="B36" s="24"/>
+      <c r="A36" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>180</v>
+      </c>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
       <c r="F36" s="13"/>
@@ -6462,7 +6472,9 @@
       <c r="H36" s="13"/>
       <c r="I36" s="13"/>
       <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
+      <c r="K36" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="L36" s="13"/>
       <c r="M36" s="14"/>
       <c r="N36" s="13"/>
@@ -6499,7 +6511,9 @@
       <c r="AS36" s="13"/>
       <c r="AT36" s="13"/>
       <c r="AU36" s="13"/>
-      <c r="AV36" s="13"/>
+      <c r="AV36" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="AW36" s="13"/>
       <c r="AX36" s="13"/>
       <c r="AY36" s="13"/>
@@ -6515,8 +6529,12 @@
       <c r="BI36" s="13"/>
       <c r="BJ36" s="13"/>
       <c r="BK36" s="13"/>
-      <c r="BL36" s="13"/>
-      <c r="BM36" s="13"/>
+      <c r="BL36" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="BM36" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="BN36" s="13"/>
       <c r="BO36" s="13"/>
       <c r="BP36" s="13"/>
@@ -6527,11 +6545,15 @@
       <c r="BU36" s="13"/>
       <c r="BV36" s="13"/>
       <c r="BW36" s="13"/>
-      <c r="BX36" s="13"/>
+      <c r="BX36" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="BY36" s="13"/>
       <c r="BZ36" s="13"/>
       <c r="CA36" s="13"/>
-      <c r="CB36" s="13"/>
+      <c r="CB36" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="CC36" s="13"/>
       <c r="CD36" s="13"/>
       <c r="CE36" s="13"/>
@@ -6551,7 +6573,9 @@
       <c r="CS36" s="13"/>
       <c r="CT36" s="13"/>
       <c r="CU36" s="13"/>
-      <c r="CV36" s="13"/>
+      <c r="CV36" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="CW36" s="13"/>
       <c r="CX36" s="13"/>
       <c r="CY36" s="13"/>
@@ -6570,7 +6594,9 @@
       <c r="DL36" s="13"/>
       <c r="DM36" s="13"/>
       <c r="DN36" s="13"/>
-      <c r="DO36" s="13"/>
+      <c r="DO36" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="DP36" s="13"/>
       <c r="DQ36" s="13"/>
     </row>

</xml_diff>

<commit_message>
Added a template showcasing Avro processors
</commit_message>
<xml_diff>
--- a/NiFi Templates.xlsx
+++ b/NiFi Templates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="18420" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="16640" windowHeight="16820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="183">
   <si>
     <t>Template Name:</t>
   </si>
@@ -582,9 +582,6 @@
     <t>WebCrawler</t>
   </si>
   <si>
-    <t>A template that takes in an initial seed URL scraps the contents of the site for more URLs. For each URL it will extract lines which match specific phrases ("nifi" in the example) email the flowfile to an address. Also it bundles together websites then compresses and puts them to a local folder.</t>
-  </si>
-  <si>
     <t>Syslog_Hbase</t>
   </si>
   <si>
@@ -609,10 +606,22 @@
     <t>This template is an example of how ListSFTP and FetchSFTP work together to create a list of files on a remote system and then decide which files the user wants to pull from the remote system.</t>
   </si>
   <si>
-    <t>PostHTTP Content-Type</t>
+    <t>Sample flow to specify a PostHTTP Content-Type by updating the mime.type on a FlowFile.  These flowfile requests are received by a HandleHttpResponse and a logging of the associated attributes is performed to view how an endpoint would receive the specified headers and content.</t>
   </si>
   <si>
-    <t>Sample flow to specify a PostHTTP Content-Type by updating the mime.type on a FlowFile.  These flowfile requests are received by a HandleHttpResponse and a logging of the associated attributes is performed to view how an endpoint would receive the specified headers and content.</t>
+    <t>PostHTTP_Content-Type</t>
+  </si>
+  <si>
+    <t>Convert_To_Avro_From_CSV_and_JSON</t>
+  </si>
+  <si>
+    <t>A template that takes in an initial seed URL scraps the contents of the site for more URLs. For each URL it will extract lines which match specific phrases ("nifi" in the example) email the flowfile to an address.
+Also it bundles together websites then compresses and puts them to a local folder.
+Note: This template requires a DistributedMapCacheServer with default values to run. It is not included because at the time of creation there was no way to explicitly include a controller service with no processors referring to it.</t>
+  </si>
+  <si>
+    <t>This flow takes in data from a random user generator using GetHTTP in two different formats, CSV and JSON. It then converts the data into Avro (JSON is massaged first) then split and converted to JSON. 
+This template is purely to showcase the different Avro related processors and isn't demonstrating one specific use-case.</t>
   </si>
 </sst>
 </file>
@@ -1391,10 +1400,10 @@
   <dimension ref="A1:DR164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="DE36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="DH37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="DO36" sqref="DO36"/>
+      <selection pane="bottomRight" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1466,11 +1475,11 @@
       </c>
       <c r="R1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T1">
         <f t="shared" si="1"/>
@@ -1478,11 +1487,11 @@
       </c>
       <c r="U1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W1">
         <f t="shared" si="1"/>
@@ -1518,7 +1527,7 @@
       </c>
       <c r="AE1">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AF1">
         <f t="shared" si="1"/>
@@ -1614,7 +1623,7 @@
       </c>
       <c r="BC1">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BD1">
         <f t="shared" si="1"/>
@@ -1702,7 +1711,7 @@
       </c>
       <c r="BY1">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="BZ1">
         <f t="shared" si="1"/>
@@ -1834,7 +1843,7 @@
       </c>
       <c r="DF1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DG1">
         <f t="shared" si="2"/>
@@ -1842,7 +1851,7 @@
       </c>
       <c r="DH1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DI1">
         <f t="shared" si="2"/>
@@ -1870,7 +1879,7 @@
       </c>
       <c r="DO1">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="DP1">
         <f t="shared" si="2"/>
@@ -5732,12 +5741,12 @@
       <c r="DP30" s="13"/>
       <c r="DQ30" s="13"/>
     </row>
-    <row r="31" spans="1:121" ht="90">
+    <row r="31" spans="1:121" ht="165">
       <c r="A31" s="16" t="s">
         <v>169</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -5892,10 +5901,10 @@
     </row>
     <row r="32" spans="1:121" ht="72" customHeight="1">
       <c r="A32" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="B32" s="24" t="s">
         <v>171</v>
-      </c>
-      <c r="B32" s="24" t="s">
-        <v>172</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
@@ -6028,10 +6037,10 @@
     </row>
     <row r="33" spans="1:121" ht="72" customHeight="1">
       <c r="A33" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="B33" s="24" t="s">
         <v>173</v>
-      </c>
-      <c r="B33" s="24" t="s">
-        <v>174</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
@@ -6162,10 +6171,10 @@
     </row>
     <row r="34" spans="1:121" ht="72" customHeight="1">
       <c r="A34" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="B34" s="24" t="s">
         <v>175</v>
-      </c>
-      <c r="B34" s="24" t="s">
-        <v>176</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="18"/>
@@ -6304,10 +6313,10 @@
     </row>
     <row r="35" spans="1:121" ht="72" customHeight="1">
       <c r="A35" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="B35" s="24" t="s">
         <v>177</v>
-      </c>
-      <c r="B35" s="24" t="s">
-        <v>178</v>
       </c>
       <c r="D35" s="18"/>
       <c r="E35" s="18"/>
@@ -6463,7 +6472,7 @@
         <v>179</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
@@ -6601,8 +6610,12 @@
       <c r="DQ36" s="13"/>
     </row>
     <row r="37" spans="1:121" ht="72" customHeight="1">
-      <c r="A37" s="16"/>
-      <c r="B37" s="24"/>
+      <c r="A37" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>182</v>
+      </c>
       <c r="D37" s="18"/>
       <c r="E37" s="18"/>
       <c r="F37" s="13"/>
@@ -6617,11 +6630,19 @@
       <c r="O37" s="13"/>
       <c r="P37" s="13"/>
       <c r="Q37" s="13"/>
-      <c r="R37" s="13"/>
-      <c r="S37" s="13"/>
+      <c r="R37" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="S37" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="T37" s="13"/>
-      <c r="U37" s="13"/>
-      <c r="V37" s="13"/>
+      <c r="U37" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="V37" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="W37" s="13"/>
       <c r="X37" s="13"/>
       <c r="Y37" s="13"/>
@@ -6630,7 +6651,9 @@
       <c r="AB37" s="13"/>
       <c r="AC37" s="13"/>
       <c r="AD37" s="13"/>
-      <c r="AE37" s="13"/>
+      <c r="AE37" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="AF37" s="13"/>
       <c r="AG37" s="13"/>
       <c r="AH37" s="13"/>
@@ -6654,7 +6677,9 @@
       <c r="AZ37" s="13"/>
       <c r="BA37" s="13"/>
       <c r="BB37" s="13"/>
-      <c r="BC37" s="13"/>
+      <c r="BC37" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="BD37" s="13"/>
       <c r="BE37" s="13"/>
       <c r="BF37" s="13"/>
@@ -6676,7 +6701,9 @@
       <c r="BV37" s="13"/>
       <c r="BW37" s="13"/>
       <c r="BX37" s="13"/>
-      <c r="BY37" s="13"/>
+      <c r="BY37" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="BZ37" s="13"/>
       <c r="CA37" s="13"/>
       <c r="CB37" s="13"/>
@@ -6709,16 +6736,22 @@
       <c r="DC37" s="13"/>
       <c r="DD37" s="13"/>
       <c r="DE37" s="13"/>
-      <c r="DF37" s="13"/>
+      <c r="DF37" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="DG37" s="13"/>
-      <c r="DH37" s="13"/>
+      <c r="DH37" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="DI37" s="13"/>
       <c r="DJ37" s="13"/>
       <c r="DK37" s="13"/>
       <c r="DL37" s="13"/>
       <c r="DM37" s="13"/>
       <c r="DN37" s="13"/>
-      <c r="DO37" s="13"/>
+      <c r="DO37" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="DP37" s="13"/>
       <c r="DQ37" s="13"/>
     </row>
@@ -19846,6 +19879,9 @@
     <mergeCell ref="N9:DQ9"/>
     <mergeCell ref="D2:L2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A37" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Changing excel to show that DistributedMapCacheServer isn't included in Webcrawler but is needed
</commit_message>
<xml_diff>
--- a/NiFi Templates.xlsx
+++ b/NiFi Templates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="16640" windowHeight="16820" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="28820" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="184">
   <si>
     <t>Template Name:</t>
   </si>
@@ -348,51 +348,6 @@
     <t xml:space="preserve">PutHBaseCell   </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">This chart list available templates and indicates what </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Processors</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> are used in those templates.  If a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Controller Service</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is marked for a template, that indicates that the template has a dependency on that Controller service existing.</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">HBase_1_1_2_ClientService   </t>
   </si>
   <si>
@@ -623,12 +578,20 @@
     <t>This flow takes in data from a random user generator using GetHTTP in two different formats, CSV and JSON. It then converts the data into Avro (JSON is massaged first) then split and converted to JSON. 
 This template is purely to showcase the different Avro related processors and isn't demonstrating one specific use-case.</t>
   </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This chart list available templates and indicates what Processors are used in those templates.  If a Controller Service is marked for a template, that indicates that the template has a dependency on that Controller service existing.
+X = Included in template
+* = Depended on by template (used when controller services tasks aren't directly included) </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -659,14 +622,6 @@
     <font>
       <b/>
       <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -821,88 +776,88 @@
   </borders>
   <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -955,7 +910,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1400,10 +1355,10 @@
   <dimension ref="A1:DR164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="DH37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B39" sqref="B39"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1419,7 +1374,7 @@
   <sheetData>
     <row r="1" spans="1:122" ht="16" thickBot="1">
       <c r="B1" s="26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D1">
         <f>COUNTIFS(D10:D300,"X")</f>
@@ -1435,7 +1390,7 @@
       </c>
       <c r="G1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H1">
         <f t="shared" si="0"/>
@@ -1892,7 +1847,7 @@
     </row>
     <row r="2" spans="1:122" s="5" customFormat="1" ht="48" customHeight="1" thickBot="1">
       <c r="A2" s="27" t="s">
-        <v>109</v>
+        <v>183</v>
       </c>
       <c r="B2" s="28"/>
       <c r="C2" s="19"/>
@@ -2025,7 +1980,7 @@
       <c r="B3" s="28"/>
       <c r="C3" s="20"/>
       <c r="D3" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>2</v>
@@ -2043,7 +1998,7 @@
         <v>6</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>7</v>
@@ -2053,7 +2008,7 @@
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>11</v>
@@ -2086,7 +2041,7 @@
         <v>20</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Z3" s="1" t="s">
         <v>21</v>
@@ -2131,7 +2086,7 @@
         <v>38</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AO3" s="1" t="s">
         <v>39</v>
@@ -2152,7 +2107,7 @@
         <v>43</v>
       </c>
       <c r="AU3" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AV3" s="1" t="s">
         <v>44</v>
@@ -2167,7 +2122,7 @@
         <v>47</v>
       </c>
       <c r="AZ3" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="BA3" s="1" t="s">
         <v>48</v>
@@ -2236,7 +2191,7 @@
         <v>67</v>
       </c>
       <c r="BW3" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="BX3" s="1" t="s">
         <v>68</v>
@@ -2254,13 +2209,13 @@
         <v>72</v>
       </c>
       <c r="CC3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="CD3" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="CD3" s="1" t="s">
+      <c r="CE3" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="CE3" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="CF3" s="1" t="s">
         <v>73</v>
@@ -2275,7 +2230,7 @@
         <v>108</v>
       </c>
       <c r="CJ3" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="CK3" s="1" t="s">
         <v>76</v>
@@ -2329,7 +2284,7 @@
         <v>91</v>
       </c>
       <c r="DB3" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="DC3" s="1" t="s">
         <v>92</v>
@@ -2341,13 +2296,13 @@
         <v>94</v>
       </c>
       <c r="DF3" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="DG3" s="1" t="s">
         <v>95</v>
       </c>
       <c r="DH3" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="DI3" s="1" t="s">
         <v>96</v>
@@ -2359,7 +2314,7 @@
         <v>98</v>
       </c>
       <c r="DL3" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="DM3" s="1" t="s">
         <v>99</v>
@@ -2839,10 +2794,10 @@
     </row>
     <row r="10" spans="1:122" ht="120">
       <c r="A10" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
@@ -3001,10 +2956,10 @@
     </row>
     <row r="11" spans="1:122" ht="90">
       <c r="A11" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
@@ -3139,10 +3094,10 @@
     </row>
     <row r="12" spans="1:122" ht="72" customHeight="1">
       <c r="A12" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="24" t="s">
         <v>113</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>114</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
@@ -3273,10 +3228,10 @@
     </row>
     <row r="13" spans="1:122" ht="72" customHeight="1">
       <c r="A13" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
@@ -3409,10 +3364,10 @@
     </row>
     <row r="14" spans="1:122" ht="90">
       <c r="A14" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
@@ -3541,10 +3496,10 @@
     </row>
     <row r="15" spans="1:122" ht="90">
       <c r="A15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="24" t="s">
         <v>120</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>121</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
@@ -3683,10 +3638,10 @@
     </row>
     <row r="16" spans="1:122" ht="72" customHeight="1">
       <c r="A16" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
@@ -3821,10 +3776,10 @@
     </row>
     <row r="17" spans="1:121" ht="120">
       <c r="A17" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="24" t="s">
         <v>124</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>125</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
@@ -3957,10 +3912,10 @@
     </row>
     <row r="18" spans="1:121" ht="72" customHeight="1">
       <c r="A18" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
@@ -4109,10 +4064,10 @@
     </row>
     <row r="19" spans="1:121" ht="72" customHeight="1">
       <c r="A19" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="18"/>
@@ -4241,10 +4196,10 @@
     </row>
     <row r="20" spans="1:121" ht="90">
       <c r="A20" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D20" s="18"/>
       <c r="E20" s="18"/>
@@ -4371,10 +4326,10 @@
     </row>
     <row r="21" spans="1:121" ht="72" customHeight="1">
       <c r="A21" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B21" s="24" t="s">
         <v>132</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>133</v>
       </c>
       <c r="D21" s="18"/>
       <c r="E21" s="18"/>
@@ -4505,10 +4460,10 @@
     </row>
     <row r="22" spans="1:121" ht="105">
       <c r="A22" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22" s="24" t="s">
         <v>134</v>
-      </c>
-      <c r="B22" s="24" t="s">
-        <v>135</v>
       </c>
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
@@ -4643,10 +4598,10 @@
     </row>
     <row r="23" spans="1:121" ht="105">
       <c r="A23" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" s="24" t="s">
         <v>137</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>138</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
@@ -4779,10 +4734,10 @@
     </row>
     <row r="24" spans="1:121" ht="120">
       <c r="A24" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B24" s="24" t="s">
         <v>139</v>
-      </c>
-      <c r="B24" s="24" t="s">
-        <v>140</v>
       </c>
       <c r="D24" s="18"/>
       <c r="E24" s="18"/>
@@ -4911,10 +4866,10 @@
     </row>
     <row r="25" spans="1:121" ht="75">
       <c r="A25" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B25" s="24" t="s">
         <v>141</v>
-      </c>
-      <c r="B25" s="24" t="s">
-        <v>142</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="18"/>
@@ -5045,10 +5000,10 @@
     </row>
     <row r="26" spans="1:121" ht="240">
       <c r="A26" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B26" s="24" t="s">
         <v>143</v>
-      </c>
-      <c r="B26" s="24" t="s">
-        <v>144</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
@@ -5185,10 +5140,10 @@
     </row>
     <row r="27" spans="1:121" ht="330">
       <c r="A27" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B27" s="24" t="s">
         <v>145</v>
-      </c>
-      <c r="B27" s="24" t="s">
-        <v>146</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="18"/>
@@ -5319,10 +5274,10 @@
     </row>
     <row r="28" spans="1:121" ht="409">
       <c r="A28" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B28" s="24" t="s">
         <v>148</v>
-      </c>
-      <c r="B28" s="24" t="s">
-        <v>149</v>
       </c>
       <c r="D28" s="18"/>
       <c r="E28" s="18"/>
@@ -5465,10 +5420,10 @@
     </row>
     <row r="29" spans="1:121" ht="72" customHeight="1">
       <c r="A29" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="B29" s="24" t="s">
         <v>164</v>
-      </c>
-      <c r="B29" s="24" t="s">
-        <v>165</v>
       </c>
       <c r="D29" s="18"/>
       <c r="E29" s="18"/>
@@ -5601,10 +5556,10 @@
     </row>
     <row r="30" spans="1:121" ht="105">
       <c r="A30" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B30" s="24" t="s">
         <v>166</v>
-      </c>
-      <c r="B30" s="24" t="s">
-        <v>167</v>
       </c>
       <c r="D30" s="18"/>
       <c r="E30" s="18"/>
@@ -5743,16 +5698,16 @@
     </row>
     <row r="31" spans="1:121" ht="165">
       <c r="A31" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
       <c r="F31" s="13"/>
       <c r="G31" s="13" t="s">
-        <v>27</v>
+        <v>182</v>
       </c>
       <c r="H31" s="13" t="s">
         <v>27</v>
@@ -5901,10 +5856,10 @@
     </row>
     <row r="32" spans="1:121" ht="72" customHeight="1">
       <c r="A32" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="B32" s="24" t="s">
         <v>170</v>
-      </c>
-      <c r="B32" s="24" t="s">
-        <v>171</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
@@ -6037,10 +5992,10 @@
     </row>
     <row r="33" spans="1:121" ht="72" customHeight="1">
       <c r="A33" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="B33" s="24" t="s">
         <v>172</v>
-      </c>
-      <c r="B33" s="24" t="s">
-        <v>173</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
@@ -6171,10 +6126,10 @@
     </row>
     <row r="34" spans="1:121" ht="72" customHeight="1">
       <c r="A34" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="B34" s="24" t="s">
         <v>174</v>
-      </c>
-      <c r="B34" s="24" t="s">
-        <v>175</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="18"/>
@@ -6313,10 +6268,10 @@
     </row>
     <row r="35" spans="1:121" ht="72" customHeight="1">
       <c r="A35" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="B35" s="24" t="s">
         <v>176</v>
-      </c>
-      <c r="B35" s="24" t="s">
-        <v>177</v>
       </c>
       <c r="D35" s="18"/>
       <c r="E35" s="18"/>
@@ -6469,10 +6424,10 @@
     </row>
     <row r="36" spans="1:121" ht="72" customHeight="1">
       <c r="A36" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
@@ -6611,10 +6566,10 @@
     </row>
     <row r="37" spans="1:121" ht="72" customHeight="1">
       <c r="A37" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D37" s="18"/>
       <c r="E37" s="18"/>

</xml_diff>

<commit_message>
Added a MongoDB template
</commit_message>
<xml_diff>
--- a/NiFi Templates.xlsx
+++ b/NiFi Templates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="28820" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="-50220" yWindow="-10540" windowWidth="48540" windowHeight="27440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="186">
   <si>
     <t>Template Name:</t>
   </si>
@@ -585,6 +585,12 @@
     <t xml:space="preserve">This chart list available templates and indicates what Processors are used in those templates.  If a Controller Service is marked for a template, that indicates that the template has a dependency on that Controller service existing.
 X = Included in template
 * = Depended on by template (used when controller services tasks aren't directly included) </t>
+  </si>
+  <si>
+    <t>MongoDB Get and Put Example</t>
+  </si>
+  <si>
+    <t>This template shows a basic configuration of the GetMongo and PutMongo processors. This template assumes you have a mongo db instance running with a test db and restaurant collection within test.</t>
   </si>
 </sst>
 </file>
@@ -1355,10 +1361,10 @@
   <dimension ref="A1:DR164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="AU38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:B3"/>
+      <selection pane="bottomRight" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1550,7 +1556,7 @@
       </c>
       <c r="AV1">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AW1">
         <f t="shared" si="1"/>
@@ -1594,7 +1600,7 @@
       </c>
       <c r="BG1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH1">
         <f t="shared" si="1"/>
@@ -1726,7 +1732,7 @@
       </c>
       <c r="CN1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CO1">
         <f t="shared" si="2"/>
@@ -1758,7 +1764,7 @@
       </c>
       <c r="CV1">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="CW1">
         <f t="shared" si="2"/>
@@ -1834,7 +1840,7 @@
       </c>
       <c r="DO1">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="DP1">
         <f t="shared" si="2"/>
@@ -6711,8 +6717,12 @@
       <c r="DQ37" s="13"/>
     </row>
     <row r="38" spans="1:121" ht="72" customHeight="1">
-      <c r="A38" s="16"/>
-      <c r="B38" s="24"/>
+      <c r="A38" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="B38" s="24" t="s">
+        <v>185</v>
+      </c>
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>
       <c r="F38" s="13"/>
@@ -6757,7 +6767,9 @@
       <c r="AS38" s="13"/>
       <c r="AT38" s="13"/>
       <c r="AU38" s="13"/>
-      <c r="AV38" s="13"/>
+      <c r="AV38" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="AW38" s="13"/>
       <c r="AX38" s="13"/>
       <c r="AY38" s="13"/>
@@ -6768,7 +6780,9 @@
       <c r="BD38" s="13"/>
       <c r="BE38" s="13"/>
       <c r="BF38" s="13"/>
-      <c r="BG38" s="13"/>
+      <c r="BG38" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="BH38" s="13"/>
       <c r="BI38" s="13"/>
       <c r="BJ38" s="13"/>
@@ -6801,7 +6815,9 @@
       <c r="CK38" s="13"/>
       <c r="CL38" s="13"/>
       <c r="CM38" s="13"/>
-      <c r="CN38" s="13"/>
+      <c r="CN38" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="CO38" s="13"/>
       <c r="CP38" s="13"/>
       <c r="CQ38" s="13"/>
@@ -6809,7 +6825,9 @@
       <c r="CS38" s="13"/>
       <c r="CT38" s="13"/>
       <c r="CU38" s="13"/>
-      <c r="CV38" s="13"/>
+      <c r="CV38" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="CW38" s="13"/>
       <c r="CX38" s="13"/>
       <c r="CY38" s="13"/>
@@ -6828,7 +6846,9 @@
       <c r="DL38" s="13"/>
       <c r="DM38" s="13"/>
       <c r="DN38" s="13"/>
-      <c r="DO38" s="13"/>
+      <c r="DO38" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="DP38" s="13"/>
       <c r="DQ38" s="13"/>
     </row>

</xml_diff>

<commit_message>
Added sample template to graph stock prices.  Described here: https://community.hortonworks.com/content/kbentry/8422/visualize-near-real-time-stock-price-changes-using.html
</commit_message>
<xml_diff>
--- a/NiFi Templates.xlsx
+++ b/NiFi Templates.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vlad\Dropbox\2014 - Hortonworks\Projects\HWX\nifi-templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-102400" yWindow="-15400" windowWidth="36540" windowHeight="20440" tabRatio="500"/>
+    <workbookView xWindow="-102405" yWindow="-15405" windowWidth="36540" windowHeight="20445" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="219">
   <si>
     <t>Template Name:</t>
   </si>
@@ -686,6 +691,12 @@
   <si>
     <t>PutElasticsearch</t>
   </si>
+  <si>
+    <t>Download real-time stock prices and send to HBase and Solr</t>
+  </si>
+  <si>
+    <t>Send_stock_prices_to_HBase_and_Solr</t>
+  </si>
 </sst>
 </file>
 
@@ -1137,6 +1148,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1466,24 +1480,24 @@
   <dimension ref="A1:ED164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="CL47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="CM9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="EA47" sqref="EA47"/>
+      <selection pane="bottomRight" activeCell="EA48" sqref="EA48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.5" style="8" customWidth="1"/>
-    <col min="3" max="3" width="1.83203125" style="12" customWidth="1"/>
-    <col min="4" max="13" width="4.83203125" customWidth="1"/>
-    <col min="14" max="14" width="1.6640625" style="3" customWidth="1"/>
-    <col min="15" max="133" width="4.83203125" customWidth="1"/>
-    <col min="134" max="134" width="1.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="1.875" style="12" customWidth="1"/>
+    <col min="4" max="13" width="4.875" customWidth="1"/>
+    <col min="14" max="14" width="1.625" style="3" customWidth="1"/>
+    <col min="15" max="133" width="4.875" customWidth="1"/>
+    <col min="134" max="134" width="1.625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:134" ht="16" thickBot="1">
+    <row r="1" spans="1:134" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="26" t="s">
         <v>153</v>
       </c>
@@ -1513,7 +1527,7 @@
       </c>
       <c r="J1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K1">
         <f t="shared" si="0"/>
@@ -1529,7 +1543,7 @@
       </c>
       <c r="O1">
         <f>COUNTIFS(O10:O300,"X")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P1">
         <f t="shared" ref="P1:CP1" si="1">COUNTIFS(P10:P300,"X")</f>
@@ -1605,7 +1619,7 @@
       </c>
       <c r="AH1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI1">
         <f t="shared" si="1"/>
@@ -1705,7 +1719,7 @@
       </c>
       <c r="BG1">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="BH1">
         <f t="shared" si="1"/>
@@ -1797,7 +1811,7 @@
       </c>
       <c r="CE1">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="CF1">
         <f t="shared" si="1"/>
@@ -1853,7 +1867,7 @@
       </c>
       <c r="CT1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="CU1">
         <f t="shared" si="2"/>
@@ -1885,7 +1899,7 @@
       </c>
       <c r="DB1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="DC1">
         <f t="shared" si="2"/>
@@ -1953,7 +1967,7 @@
       </c>
       <c r="DT1">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="DU1">
         <f t="shared" si="2"/>
@@ -1981,7 +1995,7 @@
       </c>
       <c r="EA1">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="EB1">
         <f t="shared" si="2"/>
@@ -1992,7 +2006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:134" s="5" customFormat="1" ht="48" customHeight="1" thickBot="1">
+    <row r="2" spans="1:134" s="5" customFormat="1" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="29" t="s">
         <v>183</v>
       </c>
@@ -2134,7 +2148,7 @@
       <c r="EC2" s="32"/>
       <c r="ED2" s="6"/>
     </row>
-    <row r="3" spans="1:134" s="1" customFormat="1" ht="221" customHeight="1" thickTop="1">
+    <row r="3" spans="1:134" s="1" customFormat="1" ht="221.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30"/>
       <c r="B3" s="30"/>
       <c r="C3" s="20"/>
@@ -2528,11 +2542,11 @@
       </c>
       <c r="ED3" s="4"/>
     </row>
-    <row r="4" spans="1:134" s="3" customFormat="1" ht="8" customHeight="1">
+    <row r="4" spans="1:134" s="3" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
       <c r="C4" s="12"/>
     </row>
-    <row r="5" spans="1:134">
+    <row r="5" spans="1:134" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>25</v>
       </c>
@@ -2620,7 +2634,7 @@
       <c r="CA5" s="10"/>
       <c r="CB5" s="10"/>
     </row>
-    <row r="6" spans="1:134">
+    <row r="6" spans="1:134" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>26</v>
       </c>
@@ -2714,7 +2728,7 @@
       <c r="CA6" s="10"/>
       <c r="CB6" s="10"/>
     </row>
-    <row r="7" spans="1:134">
+    <row r="7" spans="1:134" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>28</v>
       </c>
@@ -2808,7 +2822,7 @@
       <c r="CA7" s="10"/>
       <c r="CB7" s="10"/>
     </row>
-    <row r="8" spans="1:134" s="3" customFormat="1" ht="7" customHeight="1" thickBot="1">
+    <row r="8" spans="1:134" s="3" customFormat="1" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
       <c r="C8" s="12"/>
       <c r="D8" s="11"/>
@@ -2889,7 +2903,7 @@
       <c r="CA8" s="11"/>
       <c r="CB8" s="11"/>
     </row>
-    <row r="9" spans="1:134" ht="25" customHeight="1" thickTop="1">
+    <row r="9" spans="1:134" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>0</v>
       </c>
@@ -3027,7 +3041,7 @@
       <c r="EB9" s="34"/>
       <c r="EC9" s="34"/>
     </row>
-    <row r="10" spans="1:134" ht="120">
+    <row r="10" spans="1:134" ht="126" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>110</v>
       </c>
@@ -3201,7 +3215,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:134" ht="90">
+    <row r="11" spans="1:134" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>111</v>
       </c>
@@ -3351,7 +3365,7 @@
       <c r="EB11" s="13"/>
       <c r="EC11" s="13"/>
     </row>
-    <row r="12" spans="1:134" ht="72" customHeight="1">
+    <row r="12" spans="1:134" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>112</v>
       </c>
@@ -3497,7 +3511,7 @@
       <c r="EB12" s="13"/>
       <c r="EC12" s="13"/>
     </row>
-    <row r="13" spans="1:134" ht="72" customHeight="1">
+    <row r="13" spans="1:134" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>115</v>
       </c>
@@ -3645,7 +3659,7 @@
       <c r="EB13" s="13"/>
       <c r="EC13" s="13"/>
     </row>
-    <row r="14" spans="1:134" ht="90">
+    <row r="14" spans="1:134" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>116</v>
       </c>
@@ -3789,7 +3803,7 @@
       <c r="EB14" s="13"/>
       <c r="EC14" s="13"/>
     </row>
-    <row r="15" spans="1:134" ht="90">
+    <row r="15" spans="1:134" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>119</v>
       </c>
@@ -3943,7 +3957,7 @@
       <c r="EB15" s="13"/>
       <c r="EC15" s="13"/>
     </row>
-    <row r="16" spans="1:134" ht="72" customHeight="1">
+    <row r="16" spans="1:134" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>122</v>
       </c>
@@ -4093,7 +4107,7 @@
       <c r="EB16" s="13"/>
       <c r="EC16" s="13"/>
     </row>
-    <row r="17" spans="1:133" ht="120">
+    <row r="17" spans="1:133" ht="126" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>123</v>
       </c>
@@ -4241,7 +4255,7 @@
       <c r="EB17" s="13"/>
       <c r="EC17" s="13"/>
     </row>
-    <row r="18" spans="1:133" ht="72" customHeight="1">
+    <row r="18" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>126</v>
       </c>
@@ -4405,7 +4419,7 @@
       <c r="EB18" s="13"/>
       <c r="EC18" s="13"/>
     </row>
-    <row r="19" spans="1:133" ht="72" customHeight="1">
+    <row r="19" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>127</v>
       </c>
@@ -4549,7 +4563,7 @@
       <c r="EB19" s="13"/>
       <c r="EC19" s="13"/>
     </row>
-    <row r="20" spans="1:133" ht="90">
+    <row r="20" spans="1:133" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>128</v>
       </c>
@@ -4691,7 +4705,7 @@
       <c r="EB20" s="13"/>
       <c r="EC20" s="13"/>
     </row>
-    <row r="21" spans="1:133" ht="72" customHeight="1">
+    <row r="21" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>131</v>
       </c>
@@ -4837,7 +4851,7 @@
       <c r="EB21" s="13"/>
       <c r="EC21" s="13"/>
     </row>
-    <row r="22" spans="1:133" ht="105">
+    <row r="22" spans="1:133" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>133</v>
       </c>
@@ -4987,7 +5001,7 @@
       <c r="EB22" s="13"/>
       <c r="EC22" s="13"/>
     </row>
-    <row r="23" spans="1:133" ht="105">
+    <row r="23" spans="1:133" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>136</v>
       </c>
@@ -5135,7 +5149,7 @@
       <c r="EB23" s="13"/>
       <c r="EC23" s="13"/>
     </row>
-    <row r="24" spans="1:133" ht="120">
+    <row r="24" spans="1:133" ht="126" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>138</v>
       </c>
@@ -5279,7 +5293,7 @@
       <c r="EB24" s="13"/>
       <c r="EC24" s="13"/>
     </row>
-    <row r="25" spans="1:133" ht="75">
+    <row r="25" spans="1:133" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>140</v>
       </c>
@@ -5425,7 +5439,7 @@
       <c r="EB25" s="13"/>
       <c r="EC25" s="13"/>
     </row>
-    <row r="26" spans="1:133" ht="240">
+    <row r="26" spans="1:133" ht="283.5" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>142</v>
       </c>
@@ -5577,7 +5591,7 @@
       <c r="EB26" s="13"/>
       <c r="EC26" s="13"/>
     </row>
-    <row r="27" spans="1:133" ht="330">
+    <row r="27" spans="1:133" ht="346.5" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>144</v>
       </c>
@@ -5723,7 +5737,7 @@
       <c r="EB27" s="13"/>
       <c r="EC27" s="13"/>
     </row>
-    <row r="28" spans="1:133" ht="409">
+    <row r="28" spans="1:133" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>147</v>
       </c>
@@ -5881,7 +5895,7 @@
       <c r="EB28" s="13"/>
       <c r="EC28" s="13"/>
     </row>
-    <row r="29" spans="1:133" ht="72" customHeight="1">
+    <row r="29" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>163</v>
       </c>
@@ -6029,7 +6043,7 @@
       <c r="EB29" s="13"/>
       <c r="EC29" s="13"/>
     </row>
-    <row r="30" spans="1:133" ht="105">
+    <row r="30" spans="1:133" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>165</v>
       </c>
@@ -6183,7 +6197,7 @@
       <c r="EB30" s="13"/>
       <c r="EC30" s="13"/>
     </row>
-    <row r="31" spans="1:133" ht="165">
+    <row r="31" spans="1:133" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>168</v>
       </c>
@@ -6353,7 +6367,7 @@
       <c r="EB31" s="13"/>
       <c r="EC31" s="13"/>
     </row>
-    <row r="32" spans="1:133" ht="72" customHeight="1">
+    <row r="32" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>169</v>
       </c>
@@ -6501,7 +6515,7 @@
       <c r="EB32" s="13"/>
       <c r="EC32" s="13"/>
     </row>
-    <row r="33" spans="1:133" ht="72" customHeight="1">
+    <row r="33" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
         <v>171</v>
       </c>
@@ -6647,7 +6661,7 @@
       <c r="EB33" s="13"/>
       <c r="EC33" s="13"/>
     </row>
-    <row r="34" spans="1:133" ht="72" customHeight="1">
+    <row r="34" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>173</v>
       </c>
@@ -6801,7 +6815,7 @@
       <c r="EB34" s="13"/>
       <c r="EC34" s="13"/>
     </row>
-    <row r="35" spans="1:133" ht="72" customHeight="1">
+    <row r="35" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>175</v>
       </c>
@@ -6969,7 +6983,7 @@
       <c r="EB35" s="13"/>
       <c r="EC35" s="13"/>
     </row>
-    <row r="36" spans="1:133" ht="72" customHeight="1">
+    <row r="36" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>178</v>
       </c>
@@ -7123,7 +7137,7 @@
       <c r="EB36" s="13"/>
       <c r="EC36" s="13"/>
     </row>
-    <row r="37" spans="1:133" ht="72" customHeight="1">
+    <row r="37" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>179</v>
       </c>
@@ -7281,7 +7295,7 @@
       <c r="EB37" s="13"/>
       <c r="EC37" s="13"/>
     </row>
-    <row r="38" spans="1:133" ht="72" customHeight="1">
+    <row r="38" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
         <v>184</v>
       </c>
@@ -7429,7 +7443,7 @@
       <c r="EB38" s="13"/>
       <c r="EC38" s="13"/>
     </row>
-    <row r="39" spans="1:133" ht="72" customHeight="1">
+    <row r="39" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>186</v>
       </c>
@@ -7577,7 +7591,7 @@
       <c r="EB39" s="13"/>
       <c r="EC39" s="13"/>
     </row>
-    <row r="40" spans="1:133" ht="72" customHeight="1">
+    <row r="40" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>190</v>
       </c>
@@ -7743,7 +7757,7 @@
       <c r="EB40" s="13"/>
       <c r="EC40" s="13"/>
     </row>
-    <row r="41" spans="1:133" ht="72" customHeight="1">
+    <row r="41" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>193</v>
       </c>
@@ -7895,7 +7909,7 @@
       <c r="EB41" s="13"/>
       <c r="EC41" s="13"/>
     </row>
-    <row r="42" spans="1:133" ht="72" customHeight="1">
+    <row r="42" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>195</v>
       </c>
@@ -8047,7 +8061,7 @@
       <c r="EB42" s="13"/>
       <c r="EC42" s="13"/>
     </row>
-    <row r="43" spans="1:133" ht="72" customHeight="1">
+    <row r="43" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>197</v>
       </c>
@@ -8193,7 +8207,7 @@
       <c r="EB43" s="13"/>
       <c r="EC43" s="13"/>
     </row>
-    <row r="44" spans="1:133" ht="72" customHeight="1">
+    <row r="44" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>199</v>
       </c>
@@ -8341,7 +8355,7 @@
       <c r="EB44" s="13"/>
       <c r="EC44" s="13"/>
     </row>
-    <row r="45" spans="1:133" ht="72" customHeight="1">
+    <row r="45" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>204</v>
       </c>
@@ -8497,7 +8511,7 @@
       <c r="EB45" s="13"/>
       <c r="EC45" s="13"/>
     </row>
-    <row r="46" spans="1:133" ht="72" customHeight="1">
+    <row r="46" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>209</v>
       </c>
@@ -8645,7 +8659,7 @@
       <c r="EB46" s="13"/>
       <c r="EC46" s="13"/>
     </row>
-    <row r="47" spans="1:133" ht="72" customHeight="1">
+    <row r="47" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>213</v>
       </c>
@@ -8803,21 +8817,29 @@
       <c r="EB47" s="13"/>
       <c r="EC47" s="13"/>
     </row>
-    <row r="48" spans="1:133" ht="72" customHeight="1">
-      <c r="A48" s="16"/>
-      <c r="B48" s="24"/>
+    <row r="48" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>217</v>
+      </c>
       <c r="D48" s="18"/>
       <c r="E48" s="18"/>
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
       <c r="H48" s="13"/>
       <c r="I48" s="13"/>
-      <c r="J48" s="13"/>
+      <c r="J48" s="13" t="s">
+        <v>191</v>
+      </c>
       <c r="K48" s="13"/>
       <c r="L48" s="13"/>
       <c r="M48" s="13"/>
       <c r="N48" s="14"/>
-      <c r="O48" s="13"/>
+      <c r="O48" s="13" t="s">
+        <v>191</v>
+      </c>
       <c r="P48" s="13"/>
       <c r="Q48" s="13"/>
       <c r="R48" s="13"/>
@@ -8836,7 +8858,9 @@
       <c r="AE48" s="13"/>
       <c r="AF48" s="13"/>
       <c r="AG48" s="13"/>
-      <c r="AH48" s="13"/>
+      <c r="AH48" s="13" t="s">
+        <v>191</v>
+      </c>
       <c r="AI48" s="13"/>
       <c r="AJ48" s="13"/>
       <c r="AK48" s="13"/>
@@ -8861,7 +8885,9 @@
       <c r="BD48" s="13"/>
       <c r="BE48" s="13"/>
       <c r="BF48" s="13"/>
-      <c r="BG48" s="13"/>
+      <c r="BG48" s="13" t="s">
+        <v>191</v>
+      </c>
       <c r="BH48" s="13"/>
       <c r="BI48" s="13"/>
       <c r="BJ48" s="13"/>
@@ -8885,7 +8911,9 @@
       <c r="CB48" s="13"/>
       <c r="CC48" s="13"/>
       <c r="CD48" s="13"/>
-      <c r="CE48" s="13"/>
+      <c r="CE48" s="13" t="s">
+        <v>191</v>
+      </c>
       <c r="CF48" s="13"/>
       <c r="CG48" s="13"/>
       <c r="CH48" s="13"/>
@@ -8900,7 +8928,9 @@
       <c r="CQ48" s="13"/>
       <c r="CR48" s="13"/>
       <c r="CS48" s="13"/>
-      <c r="CT48" s="13"/>
+      <c r="CT48" s="13" t="s">
+        <v>191</v>
+      </c>
       <c r="CU48" s="13"/>
       <c r="CV48" s="13"/>
       <c r="CW48" s="13"/>
@@ -8908,7 +8938,9 @@
       <c r="CY48" s="13"/>
       <c r="CZ48" s="13"/>
       <c r="DA48" s="13"/>
-      <c r="DB48" s="13"/>
+      <c r="DB48" s="13" t="s">
+        <v>191</v>
+      </c>
       <c r="DC48" s="13"/>
       <c r="DD48" s="13"/>
       <c r="DE48" s="13"/>
@@ -8926,18 +8958,22 @@
       <c r="DQ48" s="13"/>
       <c r="DR48" s="13"/>
       <c r="DS48" s="13"/>
-      <c r="DT48" s="13"/>
+      <c r="DT48" s="13" t="s">
+        <v>191</v>
+      </c>
       <c r="DU48" s="13"/>
       <c r="DV48" s="13"/>
       <c r="DW48" s="13"/>
       <c r="DX48" s="13"/>
       <c r="DY48" s="13"/>
       <c r="DZ48" s="13"/>
-      <c r="EA48" s="13"/>
+      <c r="EA48" s="13" t="s">
+        <v>191</v>
+      </c>
       <c r="EB48" s="13"/>
       <c r="EC48" s="13"/>
     </row>
-    <row r="49" spans="1:133" ht="72" customHeight="1">
+    <row r="49" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16"/>
       <c r="B49" s="24"/>
       <c r="D49" s="18"/>
@@ -9071,7 +9107,7 @@
       <c r="EB49" s="13"/>
       <c r="EC49" s="13"/>
     </row>
-    <row r="50" spans="1:133" ht="72" customHeight="1">
+    <row r="50" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="16"/>
       <c r="B50" s="24"/>
       <c r="D50" s="18"/>
@@ -9205,7 +9241,7 @@
       <c r="EB50" s="13"/>
       <c r="EC50" s="13"/>
     </row>
-    <row r="51" spans="1:133" ht="72" customHeight="1">
+    <row r="51" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16"/>
       <c r="B51" s="24"/>
       <c r="D51" s="18"/>
@@ -9339,7 +9375,7 @@
       <c r="EB51" s="13"/>
       <c r="EC51" s="13"/>
     </row>
-    <row r="52" spans="1:133" ht="72" customHeight="1">
+    <row r="52" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="16"/>
       <c r="B52" s="24"/>
       <c r="D52" s="18"/>
@@ -9473,7 +9509,7 @@
       <c r="EB52" s="13"/>
       <c r="EC52" s="13"/>
     </row>
-    <row r="53" spans="1:133" ht="72" customHeight="1">
+    <row r="53" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16"/>
       <c r="B53" s="24"/>
       <c r="D53" s="18"/>
@@ -9607,7 +9643,7 @@
       <c r="EB53" s="13"/>
       <c r="EC53" s="13"/>
     </row>
-    <row r="54" spans="1:133" ht="72" customHeight="1">
+    <row r="54" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="16"/>
       <c r="B54" s="24"/>
       <c r="D54" s="18"/>
@@ -9741,7 +9777,7 @@
       <c r="EB54" s="13"/>
       <c r="EC54" s="13"/>
     </row>
-    <row r="55" spans="1:133" ht="72" customHeight="1">
+    <row r="55" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="16"/>
       <c r="B55" s="24"/>
       <c r="D55" s="18"/>
@@ -9875,7 +9911,7 @@
       <c r="EB55" s="13"/>
       <c r="EC55" s="13"/>
     </row>
-    <row r="56" spans="1:133" ht="72" customHeight="1">
+    <row r="56" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="16"/>
       <c r="B56" s="24"/>
       <c r="D56" s="18"/>
@@ -10009,7 +10045,7 @@
       <c r="EB56" s="13"/>
       <c r="EC56" s="13"/>
     </row>
-    <row r="57" spans="1:133" ht="72" customHeight="1">
+    <row r="57" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16"/>
       <c r="B57" s="24"/>
       <c r="D57" s="18"/>
@@ -10143,7 +10179,7 @@
       <c r="EB57" s="13"/>
       <c r="EC57" s="13"/>
     </row>
-    <row r="58" spans="1:133" ht="72" customHeight="1">
+    <row r="58" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="16"/>
       <c r="B58" s="24"/>
       <c r="D58" s="18"/>
@@ -10277,7 +10313,7 @@
       <c r="EB58" s="13"/>
       <c r="EC58" s="13"/>
     </row>
-    <row r="59" spans="1:133" ht="72" customHeight="1">
+    <row r="59" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="16"/>
       <c r="B59" s="24"/>
       <c r="D59" s="18"/>
@@ -10411,7 +10447,7 @@
       <c r="EB59" s="13"/>
       <c r="EC59" s="13"/>
     </row>
-    <row r="60" spans="1:133" ht="72" customHeight="1">
+    <row r="60" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="16"/>
       <c r="B60" s="24"/>
       <c r="D60" s="18"/>
@@ -10545,7 +10581,7 @@
       <c r="EB60" s="13"/>
       <c r="EC60" s="13"/>
     </row>
-    <row r="61" spans="1:133" ht="72" customHeight="1">
+    <row r="61" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="16"/>
       <c r="B61" s="24"/>
       <c r="D61" s="18"/>
@@ -10679,7 +10715,7 @@
       <c r="EB61" s="13"/>
       <c r="EC61" s="13"/>
     </row>
-    <row r="62" spans="1:133" ht="72" customHeight="1">
+    <row r="62" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="16"/>
       <c r="B62" s="24"/>
       <c r="D62" s="18"/>
@@ -10813,7 +10849,7 @@
       <c r="EB62" s="13"/>
       <c r="EC62" s="13"/>
     </row>
-    <row r="63" spans="1:133" ht="72" customHeight="1">
+    <row r="63" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="16"/>
       <c r="B63" s="24"/>
       <c r="D63" s="18"/>
@@ -10947,7 +10983,7 @@
       <c r="EB63" s="13"/>
       <c r="EC63" s="13"/>
     </row>
-    <row r="64" spans="1:133" ht="72" customHeight="1">
+    <row r="64" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="16"/>
       <c r="B64" s="24"/>
       <c r="D64" s="18"/>
@@ -11081,7 +11117,7 @@
       <c r="EB64" s="13"/>
       <c r="EC64" s="13"/>
     </row>
-    <row r="65" spans="1:133" ht="72" customHeight="1">
+    <row r="65" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="16"/>
       <c r="B65" s="24"/>
       <c r="D65" s="18"/>
@@ -11215,7 +11251,7 @@
       <c r="EB65" s="13"/>
       <c r="EC65" s="13"/>
     </row>
-    <row r="66" spans="1:133" ht="72" customHeight="1">
+    <row r="66" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="16"/>
       <c r="B66" s="24"/>
       <c r="D66" s="18"/>
@@ -11349,7 +11385,7 @@
       <c r="EB66" s="13"/>
       <c r="EC66" s="13"/>
     </row>
-    <row r="67" spans="1:133" ht="72" customHeight="1">
+    <row r="67" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="16"/>
       <c r="B67" s="24"/>
       <c r="D67" s="18"/>
@@ -11483,7 +11519,7 @@
       <c r="EB67" s="13"/>
       <c r="EC67" s="13"/>
     </row>
-    <row r="68" spans="1:133" ht="72" customHeight="1">
+    <row r="68" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="16"/>
       <c r="B68" s="24"/>
       <c r="D68" s="18"/>
@@ -11617,7 +11653,7 @@
       <c r="EB68" s="13"/>
       <c r="EC68" s="13"/>
     </row>
-    <row r="69" spans="1:133" ht="72" customHeight="1">
+    <row r="69" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="16"/>
       <c r="B69" s="24"/>
       <c r="D69" s="18"/>
@@ -11751,7 +11787,7 @@
       <c r="EB69" s="13"/>
       <c r="EC69" s="13"/>
     </row>
-    <row r="70" spans="1:133" ht="72" customHeight="1">
+    <row r="70" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="16"/>
       <c r="B70" s="24"/>
       <c r="D70" s="18"/>
@@ -11885,7 +11921,7 @@
       <c r="EB70" s="13"/>
       <c r="EC70" s="13"/>
     </row>
-    <row r="71" spans="1:133" ht="72" customHeight="1">
+    <row r="71" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="16"/>
       <c r="B71" s="24"/>
       <c r="D71" s="18"/>
@@ -12019,7 +12055,7 @@
       <c r="EB71" s="13"/>
       <c r="EC71" s="13"/>
     </row>
-    <row r="72" spans="1:133" ht="72" customHeight="1">
+    <row r="72" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="16"/>
       <c r="B72" s="24"/>
       <c r="D72" s="18"/>
@@ -12153,7 +12189,7 @@
       <c r="EB72" s="13"/>
       <c r="EC72" s="13"/>
     </row>
-    <row r="73" spans="1:133" ht="72" customHeight="1">
+    <row r="73" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="16"/>
       <c r="B73" s="24"/>
       <c r="D73" s="18"/>
@@ -12287,7 +12323,7 @@
       <c r="EB73" s="13"/>
       <c r="EC73" s="13"/>
     </row>
-    <row r="74" spans="1:133" ht="72" customHeight="1">
+    <row r="74" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="16"/>
       <c r="B74" s="24"/>
       <c r="D74" s="18"/>
@@ -12421,7 +12457,7 @@
       <c r="EB74" s="13"/>
       <c r="EC74" s="13"/>
     </row>
-    <row r="75" spans="1:133" ht="72" customHeight="1">
+    <row r="75" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="16"/>
       <c r="B75" s="24"/>
       <c r="D75" s="18"/>
@@ -12555,7 +12591,7 @@
       <c r="EB75" s="13"/>
       <c r="EC75" s="13"/>
     </row>
-    <row r="76" spans="1:133" ht="72" customHeight="1">
+    <row r="76" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="16"/>
       <c r="B76" s="24"/>
       <c r="D76" s="18"/>
@@ -12689,7 +12725,7 @@
       <c r="EB76" s="13"/>
       <c r="EC76" s="13"/>
     </row>
-    <row r="77" spans="1:133" ht="72" customHeight="1">
+    <row r="77" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="16"/>
       <c r="B77" s="24"/>
       <c r="D77" s="18"/>
@@ -12823,7 +12859,7 @@
       <c r="EB77" s="13"/>
       <c r="EC77" s="13"/>
     </row>
-    <row r="78" spans="1:133" ht="72" customHeight="1">
+    <row r="78" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="16"/>
       <c r="B78" s="24"/>
       <c r="D78" s="18"/>
@@ -12957,7 +12993,7 @@
       <c r="EB78" s="13"/>
       <c r="EC78" s="13"/>
     </row>
-    <row r="79" spans="1:133" ht="72" customHeight="1">
+    <row r="79" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="16"/>
       <c r="B79" s="24"/>
       <c r="D79" s="18"/>
@@ -13091,7 +13127,7 @@
       <c r="EB79" s="13"/>
       <c r="EC79" s="13"/>
     </row>
-    <row r="80" spans="1:133" ht="72" customHeight="1">
+    <row r="80" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="16"/>
       <c r="B80" s="24"/>
       <c r="D80" s="18"/>
@@ -13225,7 +13261,7 @@
       <c r="EB80" s="13"/>
       <c r="EC80" s="13"/>
     </row>
-    <row r="81" spans="1:133" ht="72" customHeight="1">
+    <row r="81" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="16"/>
       <c r="B81" s="24"/>
       <c r="D81" s="18"/>
@@ -13359,7 +13395,7 @@
       <c r="EB81" s="13"/>
       <c r="EC81" s="13"/>
     </row>
-    <row r="82" spans="1:133" ht="72" customHeight="1">
+    <row r="82" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="16"/>
       <c r="B82" s="24"/>
       <c r="D82" s="18"/>
@@ -13493,7 +13529,7 @@
       <c r="EB82" s="13"/>
       <c r="EC82" s="13"/>
     </row>
-    <row r="83" spans="1:133" ht="72" customHeight="1">
+    <row r="83" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="16"/>
       <c r="B83" s="24"/>
       <c r="D83" s="18"/>
@@ -13627,7 +13663,7 @@
       <c r="EB83" s="13"/>
       <c r="EC83" s="13"/>
     </row>
-    <row r="84" spans="1:133" ht="72" customHeight="1">
+    <row r="84" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="16"/>
       <c r="B84" s="24"/>
       <c r="D84" s="18"/>
@@ -13761,7 +13797,7 @@
       <c r="EB84" s="13"/>
       <c r="EC84" s="13"/>
     </row>
-    <row r="85" spans="1:133" ht="72" customHeight="1">
+    <row r="85" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="16"/>
       <c r="B85" s="24"/>
       <c r="D85" s="18"/>
@@ -13895,7 +13931,7 @@
       <c r="EB85" s="13"/>
       <c r="EC85" s="13"/>
     </row>
-    <row r="86" spans="1:133" ht="72" customHeight="1">
+    <row r="86" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="16"/>
       <c r="B86" s="24"/>
       <c r="D86" s="18"/>
@@ -14029,7 +14065,7 @@
       <c r="EB86" s="13"/>
       <c r="EC86" s="13"/>
     </row>
-    <row r="87" spans="1:133" ht="72" customHeight="1">
+    <row r="87" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="16"/>
       <c r="B87" s="24"/>
       <c r="D87" s="18"/>
@@ -14163,7 +14199,7 @@
       <c r="EB87" s="13"/>
       <c r="EC87" s="13"/>
     </row>
-    <row r="88" spans="1:133" ht="72" customHeight="1">
+    <row r="88" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="16"/>
       <c r="B88" s="24"/>
       <c r="D88" s="18"/>
@@ -14297,7 +14333,7 @@
       <c r="EB88" s="13"/>
       <c r="EC88" s="13"/>
     </row>
-    <row r="89" spans="1:133" ht="72" customHeight="1">
+    <row r="89" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="16"/>
       <c r="B89" s="24"/>
       <c r="D89" s="18"/>
@@ -14431,7 +14467,7 @@
       <c r="EB89" s="13"/>
       <c r="EC89" s="13"/>
     </row>
-    <row r="90" spans="1:133" ht="72" customHeight="1">
+    <row r="90" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="16"/>
       <c r="B90" s="24"/>
       <c r="D90" s="18"/>
@@ -14565,7 +14601,7 @@
       <c r="EB90" s="13"/>
       <c r="EC90" s="13"/>
     </row>
-    <row r="91" spans="1:133" ht="72" customHeight="1">
+    <row r="91" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="16"/>
       <c r="B91" s="24"/>
       <c r="D91" s="18"/>
@@ -14699,7 +14735,7 @@
       <c r="EB91" s="13"/>
       <c r="EC91" s="13"/>
     </row>
-    <row r="92" spans="1:133" ht="72" customHeight="1">
+    <row r="92" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="16"/>
       <c r="B92" s="24"/>
       <c r="D92" s="18"/>
@@ -14833,7 +14869,7 @@
       <c r="EB92" s="13"/>
       <c r="EC92" s="13"/>
     </row>
-    <row r="93" spans="1:133" ht="72" customHeight="1">
+    <row r="93" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="16"/>
       <c r="B93" s="24"/>
       <c r="D93" s="18"/>
@@ -14967,7 +15003,7 @@
       <c r="EB93" s="13"/>
       <c r="EC93" s="13"/>
     </row>
-    <row r="94" spans="1:133" ht="72" customHeight="1">
+    <row r="94" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="16"/>
       <c r="B94" s="24"/>
       <c r="D94" s="18"/>
@@ -15101,7 +15137,7 @@
       <c r="EB94" s="13"/>
       <c r="EC94" s="13"/>
     </row>
-    <row r="95" spans="1:133" ht="72" customHeight="1">
+    <row r="95" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="16"/>
       <c r="B95" s="24"/>
       <c r="D95" s="18"/>
@@ -15235,7 +15271,7 @@
       <c r="EB95" s="13"/>
       <c r="EC95" s="13"/>
     </row>
-    <row r="96" spans="1:133" ht="72" customHeight="1">
+    <row r="96" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="16"/>
       <c r="B96" s="24"/>
       <c r="D96" s="18"/>
@@ -15369,7 +15405,7 @@
       <c r="EB96" s="13"/>
       <c r="EC96" s="13"/>
     </row>
-    <row r="97" spans="1:133" ht="72" customHeight="1">
+    <row r="97" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="16"/>
       <c r="B97" s="24"/>
       <c r="D97" s="18"/>
@@ -15503,7 +15539,7 @@
       <c r="EB97" s="13"/>
       <c r="EC97" s="13"/>
     </row>
-    <row r="98" spans="1:133" ht="72" customHeight="1">
+    <row r="98" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="16"/>
       <c r="B98" s="24"/>
       <c r="D98" s="18"/>
@@ -15637,7 +15673,7 @@
       <c r="EB98" s="13"/>
       <c r="EC98" s="13"/>
     </row>
-    <row r="99" spans="1:133" ht="72" customHeight="1">
+    <row r="99" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="16"/>
       <c r="B99" s="24"/>
       <c r="D99" s="18"/>
@@ -15771,7 +15807,7 @@
       <c r="EB99" s="13"/>
       <c r="EC99" s="13"/>
     </row>
-    <row r="100" spans="1:133" ht="72" customHeight="1">
+    <row r="100" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="16"/>
       <c r="B100" s="24"/>
       <c r="D100" s="18"/>
@@ -15905,7 +15941,7 @@
       <c r="EB100" s="13"/>
       <c r="EC100" s="13"/>
     </row>
-    <row r="101" spans="1:133" ht="72" customHeight="1">
+    <row r="101" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="16"/>
       <c r="B101" s="24"/>
       <c r="D101" s="18"/>
@@ -16039,7 +16075,7 @@
       <c r="EB101" s="13"/>
       <c r="EC101" s="13"/>
     </row>
-    <row r="102" spans="1:133" ht="72" customHeight="1">
+    <row r="102" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="16"/>
       <c r="B102" s="24"/>
       <c r="D102" s="18"/>
@@ -16173,7 +16209,7 @@
       <c r="EB102" s="13"/>
       <c r="EC102" s="13"/>
     </row>
-    <row r="103" spans="1:133" ht="72" customHeight="1">
+    <row r="103" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="16"/>
       <c r="B103" s="24"/>
       <c r="D103" s="18"/>
@@ -16307,7 +16343,7 @@
       <c r="EB103" s="13"/>
       <c r="EC103" s="13"/>
     </row>
-    <row r="104" spans="1:133" ht="72" customHeight="1">
+    <row r="104" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="16"/>
       <c r="B104" s="24"/>
       <c r="D104" s="18"/>
@@ -16441,7 +16477,7 @@
       <c r="EB104" s="13"/>
       <c r="EC104" s="13"/>
     </row>
-    <row r="105" spans="1:133" ht="72" customHeight="1">
+    <row r="105" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="16"/>
       <c r="B105" s="24"/>
       <c r="D105" s="18"/>
@@ -16575,7 +16611,7 @@
       <c r="EB105" s="13"/>
       <c r="EC105" s="13"/>
     </row>
-    <row r="106" spans="1:133" ht="72" customHeight="1">
+    <row r="106" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="16"/>
       <c r="B106" s="24"/>
       <c r="D106" s="18"/>
@@ -16709,7 +16745,7 @@
       <c r="EB106" s="13"/>
       <c r="EC106" s="13"/>
     </row>
-    <row r="107" spans="1:133" ht="72" customHeight="1">
+    <row r="107" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="16"/>
       <c r="B107" s="24"/>
       <c r="D107" s="18"/>
@@ -16843,7 +16879,7 @@
       <c r="EB107" s="13"/>
       <c r="EC107" s="13"/>
     </row>
-    <row r="108" spans="1:133" ht="72" customHeight="1">
+    <row r="108" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="16"/>
       <c r="B108" s="24"/>
       <c r="D108" s="18"/>
@@ -16977,7 +17013,7 @@
       <c r="EB108" s="13"/>
       <c r="EC108" s="13"/>
     </row>
-    <row r="109" spans="1:133" ht="72" customHeight="1">
+    <row r="109" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="16"/>
       <c r="B109" s="24"/>
       <c r="D109" s="18"/>
@@ -17111,7 +17147,7 @@
       <c r="EB109" s="13"/>
       <c r="EC109" s="13"/>
     </row>
-    <row r="110" spans="1:133" ht="72" customHeight="1">
+    <row r="110" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="16"/>
       <c r="B110" s="24"/>
       <c r="D110" s="18"/>
@@ -17245,7 +17281,7 @@
       <c r="EB110" s="13"/>
       <c r="EC110" s="13"/>
     </row>
-    <row r="111" spans="1:133" ht="72" customHeight="1">
+    <row r="111" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="16"/>
       <c r="B111" s="24"/>
       <c r="D111" s="18"/>
@@ -17379,7 +17415,7 @@
       <c r="EB111" s="13"/>
       <c r="EC111" s="13"/>
     </row>
-    <row r="112" spans="1:133" ht="72" customHeight="1">
+    <row r="112" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="16"/>
       <c r="B112" s="24"/>
       <c r="D112" s="18"/>
@@ -17513,7 +17549,7 @@
       <c r="EB112" s="13"/>
       <c r="EC112" s="13"/>
     </row>
-    <row r="113" spans="1:133" ht="72" customHeight="1">
+    <row r="113" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="16"/>
       <c r="B113" s="24"/>
       <c r="D113" s="18"/>
@@ -17647,7 +17683,7 @@
       <c r="EB113" s="13"/>
       <c r="EC113" s="13"/>
     </row>
-    <row r="114" spans="1:133" ht="72" customHeight="1">
+    <row r="114" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="16"/>
       <c r="B114" s="24"/>
       <c r="D114" s="18"/>
@@ -17781,7 +17817,7 @@
       <c r="EB114" s="13"/>
       <c r="EC114" s="13"/>
     </row>
-    <row r="115" spans="1:133" ht="72" customHeight="1">
+    <row r="115" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="16"/>
       <c r="B115" s="24"/>
       <c r="D115" s="18"/>
@@ -17915,7 +17951,7 @@
       <c r="EB115" s="13"/>
       <c r="EC115" s="13"/>
     </row>
-    <row r="116" spans="1:133" ht="72" customHeight="1">
+    <row r="116" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="16"/>
       <c r="B116" s="24"/>
       <c r="D116" s="18"/>
@@ -18049,7 +18085,7 @@
       <c r="EB116" s="13"/>
       <c r="EC116" s="13"/>
     </row>
-    <row r="117" spans="1:133" ht="72" customHeight="1">
+    <row r="117" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="25"/>
       <c r="D117" s="10"/>
       <c r="E117" s="21"/>
@@ -18129,7 +18165,7 @@
       <c r="CA117" s="10"/>
       <c r="CB117" s="10"/>
     </row>
-    <row r="118" spans="1:133" ht="72" customHeight="1">
+    <row r="118" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" s="25"/>
       <c r="D118" s="10"/>
       <c r="E118" s="21"/>
@@ -18209,7 +18245,7 @@
       <c r="CA118" s="10"/>
       <c r="CB118" s="10"/>
     </row>
-    <row r="119" spans="1:133">
+    <row r="119" spans="1:133" x14ac:dyDescent="0.25">
       <c r="B119" s="25"/>
       <c r="D119" s="10"/>
       <c r="E119" s="21"/>
@@ -18289,7 +18325,7 @@
       <c r="CA119" s="10"/>
       <c r="CB119" s="10"/>
     </row>
-    <row r="120" spans="1:133">
+    <row r="120" spans="1:133" x14ac:dyDescent="0.25">
       <c r="B120" s="25"/>
       <c r="D120" s="10"/>
       <c r="E120" s="21"/>
@@ -18369,7 +18405,7 @@
       <c r="CA120" s="10"/>
       <c r="CB120" s="10"/>
     </row>
-    <row r="121" spans="1:133">
+    <row r="121" spans="1:133" x14ac:dyDescent="0.25">
       <c r="B121" s="25"/>
       <c r="D121" s="10"/>
       <c r="E121" s="21"/>
@@ -18449,7 +18485,7 @@
       <c r="CA121" s="10"/>
       <c r="CB121" s="10"/>
     </row>
-    <row r="122" spans="1:133">
+    <row r="122" spans="1:133" x14ac:dyDescent="0.25">
       <c r="B122" s="25"/>
       <c r="D122" s="10"/>
       <c r="E122" s="21"/>
@@ -18529,7 +18565,7 @@
       <c r="CA122" s="10"/>
       <c r="CB122" s="10"/>
     </row>
-    <row r="123" spans="1:133">
+    <row r="123" spans="1:133" x14ac:dyDescent="0.25">
       <c r="B123" s="25"/>
       <c r="D123" s="10"/>
       <c r="E123" s="21"/>
@@ -18609,7 +18645,7 @@
       <c r="CA123" s="10"/>
       <c r="CB123" s="10"/>
     </row>
-    <row r="124" spans="1:133">
+    <row r="124" spans="1:133" x14ac:dyDescent="0.25">
       <c r="B124" s="25"/>
       <c r="D124" s="10"/>
       <c r="E124" s="21"/>
@@ -18689,7 +18725,7 @@
       <c r="CA124" s="10"/>
       <c r="CB124" s="10"/>
     </row>
-    <row r="125" spans="1:133">
+    <row r="125" spans="1:133" x14ac:dyDescent="0.25">
       <c r="B125" s="25"/>
       <c r="D125" s="10"/>
       <c r="E125" s="21"/>
@@ -18769,7 +18805,7 @@
       <c r="CA125" s="10"/>
       <c r="CB125" s="10"/>
     </row>
-    <row r="126" spans="1:133">
+    <row r="126" spans="1:133" x14ac:dyDescent="0.25">
       <c r="B126" s="25"/>
       <c r="D126" s="10"/>
       <c r="E126" s="21"/>
@@ -18849,7 +18885,7 @@
       <c r="CA126" s="10"/>
       <c r="CB126" s="10"/>
     </row>
-    <row r="127" spans="1:133">
+    <row r="127" spans="1:133" x14ac:dyDescent="0.25">
       <c r="B127" s="25"/>
       <c r="D127" s="10"/>
       <c r="E127" s="21"/>
@@ -18929,7 +18965,7 @@
       <c r="CA127" s="10"/>
       <c r="CB127" s="10"/>
     </row>
-    <row r="128" spans="1:133">
+    <row r="128" spans="1:133" x14ac:dyDescent="0.25">
       <c r="B128" s="25"/>
       <c r="D128" s="10"/>
       <c r="E128" s="21"/>
@@ -19009,7 +19045,7 @@
       <c r="CA128" s="10"/>
       <c r="CB128" s="10"/>
     </row>
-    <row r="129" spans="2:80">
+    <row r="129" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B129" s="25"/>
       <c r="D129" s="10"/>
       <c r="E129" s="21"/>
@@ -19089,7 +19125,7 @@
       <c r="CA129" s="10"/>
       <c r="CB129" s="10"/>
     </row>
-    <row r="130" spans="2:80">
+    <row r="130" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B130" s="25"/>
       <c r="D130" s="10"/>
       <c r="E130" s="21"/>
@@ -19169,7 +19205,7 @@
       <c r="CA130" s="10"/>
       <c r="CB130" s="10"/>
     </row>
-    <row r="131" spans="2:80">
+    <row r="131" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B131" s="25"/>
       <c r="D131" s="10"/>
       <c r="E131" s="21"/>
@@ -19249,7 +19285,7 @@
       <c r="CA131" s="10"/>
       <c r="CB131" s="10"/>
     </row>
-    <row r="132" spans="2:80">
+    <row r="132" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B132" s="25"/>
       <c r="D132" s="10"/>
       <c r="E132" s="21"/>
@@ -19329,7 +19365,7 @@
       <c r="CA132" s="10"/>
       <c r="CB132" s="10"/>
     </row>
-    <row r="133" spans="2:80">
+    <row r="133" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B133" s="25"/>
       <c r="D133" s="10"/>
       <c r="E133" s="21"/>
@@ -19409,7 +19445,7 @@
       <c r="CA133" s="10"/>
       <c r="CB133" s="10"/>
     </row>
-    <row r="134" spans="2:80">
+    <row r="134" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B134" s="25"/>
       <c r="D134" s="10"/>
       <c r="E134" s="21"/>
@@ -19489,7 +19525,7 @@
       <c r="CA134" s="10"/>
       <c r="CB134" s="10"/>
     </row>
-    <row r="135" spans="2:80">
+    <row r="135" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B135" s="25"/>
       <c r="D135" s="10"/>
       <c r="E135" s="21"/>
@@ -19569,7 +19605,7 @@
       <c r="CA135" s="10"/>
       <c r="CB135" s="10"/>
     </row>
-    <row r="136" spans="2:80">
+    <row r="136" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B136" s="25"/>
       <c r="D136" s="10"/>
       <c r="E136" s="21"/>
@@ -19649,7 +19685,7 @@
       <c r="CA136" s="10"/>
       <c r="CB136" s="10"/>
     </row>
-    <row r="137" spans="2:80">
+    <row r="137" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B137" s="25"/>
       <c r="D137" s="10"/>
       <c r="E137" s="21"/>
@@ -19729,7 +19765,7 @@
       <c r="CA137" s="10"/>
       <c r="CB137" s="10"/>
     </row>
-    <row r="138" spans="2:80">
+    <row r="138" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B138" s="25"/>
       <c r="D138" s="10"/>
       <c r="E138" s="21"/>
@@ -19809,7 +19845,7 @@
       <c r="CA138" s="10"/>
       <c r="CB138" s="10"/>
     </row>
-    <row r="139" spans="2:80">
+    <row r="139" spans="2:80" x14ac:dyDescent="0.25">
       <c r="D139" s="10"/>
       <c r="E139" s="21"/>
       <c r="F139" s="10"/>
@@ -19888,7 +19924,7 @@
       <c r="CA139" s="10"/>
       <c r="CB139" s="10"/>
     </row>
-    <row r="140" spans="2:80">
+    <row r="140" spans="2:80" x14ac:dyDescent="0.25">
       <c r="D140" s="10"/>
       <c r="E140" s="21"/>
       <c r="F140" s="10"/>
@@ -19967,7 +20003,7 @@
       <c r="CA140" s="10"/>
       <c r="CB140" s="10"/>
     </row>
-    <row r="141" spans="2:80">
+    <row r="141" spans="2:80" x14ac:dyDescent="0.25">
       <c r="D141" s="10"/>
       <c r="E141" s="21"/>
       <c r="F141" s="10"/>
@@ -20046,7 +20082,7 @@
       <c r="CA141" s="10"/>
       <c r="CB141" s="10"/>
     </row>
-    <row r="142" spans="2:80">
+    <row r="142" spans="2:80" x14ac:dyDescent="0.25">
       <c r="D142" s="10"/>
       <c r="E142" s="21"/>
       <c r="F142" s="10"/>
@@ -20125,7 +20161,7 @@
       <c r="CA142" s="10"/>
       <c r="CB142" s="10"/>
     </row>
-    <row r="143" spans="2:80">
+    <row r="143" spans="2:80" x14ac:dyDescent="0.25">
       <c r="D143" s="10"/>
       <c r="E143" s="21"/>
       <c r="F143" s="10"/>
@@ -20204,7 +20240,7 @@
       <c r="CA143" s="10"/>
       <c r="CB143" s="10"/>
     </row>
-    <row r="144" spans="2:80">
+    <row r="144" spans="2:80" x14ac:dyDescent="0.25">
       <c r="D144" s="10"/>
       <c r="E144" s="21"/>
       <c r="F144" s="10"/>
@@ -20283,7 +20319,7 @@
       <c r="CA144" s="10"/>
       <c r="CB144" s="10"/>
     </row>
-    <row r="145" spans="4:80">
+    <row r="145" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D145" s="10"/>
       <c r="E145" s="21"/>
       <c r="F145" s="10"/>
@@ -20362,7 +20398,7 @@
       <c r="CA145" s="10"/>
       <c r="CB145" s="10"/>
     </row>
-    <row r="146" spans="4:80">
+    <row r="146" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D146" s="10"/>
       <c r="E146" s="21"/>
       <c r="F146" s="10"/>
@@ -20441,7 +20477,7 @@
       <c r="CA146" s="10"/>
       <c r="CB146" s="10"/>
     </row>
-    <row r="147" spans="4:80">
+    <row r="147" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D147" s="10"/>
       <c r="E147" s="21"/>
       <c r="F147" s="10"/>
@@ -20520,7 +20556,7 @@
       <c r="CA147" s="10"/>
       <c r="CB147" s="10"/>
     </row>
-    <row r="148" spans="4:80">
+    <row r="148" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D148" s="10"/>
       <c r="E148" s="21"/>
       <c r="F148" s="10"/>
@@ -20599,7 +20635,7 @@
       <c r="CA148" s="10"/>
       <c r="CB148" s="10"/>
     </row>
-    <row r="149" spans="4:80">
+    <row r="149" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D149" s="10"/>
       <c r="E149" s="21"/>
       <c r="F149" s="10"/>
@@ -20678,7 +20714,7 @@
       <c r="CA149" s="10"/>
       <c r="CB149" s="10"/>
     </row>
-    <row r="150" spans="4:80">
+    <row r="150" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D150" s="10"/>
       <c r="E150" s="21"/>
       <c r="F150" s="10"/>
@@ -20757,7 +20793,7 @@
       <c r="CA150" s="10"/>
       <c r="CB150" s="10"/>
     </row>
-    <row r="151" spans="4:80">
+    <row r="151" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D151" s="10"/>
       <c r="E151" s="21"/>
       <c r="F151" s="10"/>
@@ -20836,7 +20872,7 @@
       <c r="CA151" s="10"/>
       <c r="CB151" s="10"/>
     </row>
-    <row r="152" spans="4:80">
+    <row r="152" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D152" s="10"/>
       <c r="E152" s="21"/>
       <c r="F152" s="10"/>
@@ -20915,7 +20951,7 @@
       <c r="CA152" s="10"/>
       <c r="CB152" s="10"/>
     </row>
-    <row r="153" spans="4:80">
+    <row r="153" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D153" s="10"/>
       <c r="E153" s="21"/>
       <c r="F153" s="10"/>
@@ -20994,7 +21030,7 @@
       <c r="CA153" s="10"/>
       <c r="CB153" s="10"/>
     </row>
-    <row r="154" spans="4:80">
+    <row r="154" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D154" s="10"/>
       <c r="E154" s="21"/>
       <c r="F154" s="10"/>
@@ -21073,7 +21109,7 @@
       <c r="CA154" s="10"/>
       <c r="CB154" s="10"/>
     </row>
-    <row r="155" spans="4:80">
+    <row r="155" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D155" s="10"/>
       <c r="E155" s="21"/>
       <c r="F155" s="10"/>
@@ -21152,7 +21188,7 @@
       <c r="CA155" s="10"/>
       <c r="CB155" s="10"/>
     </row>
-    <row r="156" spans="4:80">
+    <row r="156" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D156" s="10"/>
       <c r="E156" s="21"/>
       <c r="F156" s="10"/>
@@ -21231,7 +21267,7 @@
       <c r="CA156" s="10"/>
       <c r="CB156" s="10"/>
     </row>
-    <row r="157" spans="4:80">
+    <row r="157" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D157" s="10"/>
       <c r="E157" s="21"/>
       <c r="F157" s="10"/>
@@ -21310,7 +21346,7 @@
       <c r="CA157" s="10"/>
       <c r="CB157" s="10"/>
     </row>
-    <row r="158" spans="4:80">
+    <row r="158" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D158" s="10"/>
       <c r="E158" s="21"/>
       <c r="F158" s="10"/>
@@ -21389,7 +21425,7 @@
       <c r="CA158" s="10"/>
       <c r="CB158" s="10"/>
     </row>
-    <row r="159" spans="4:80">
+    <row r="159" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D159" s="10"/>
       <c r="E159" s="21"/>
       <c r="F159" s="10"/>
@@ -21468,7 +21504,7 @@
       <c r="CA159" s="10"/>
       <c r="CB159" s="10"/>
     </row>
-    <row r="160" spans="4:80">
+    <row r="160" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D160" s="10"/>
       <c r="E160" s="21"/>
       <c r="F160" s="10"/>
@@ -21547,7 +21583,7 @@
       <c r="CA160" s="10"/>
       <c r="CB160" s="10"/>
     </row>
-    <row r="161" spans="4:80">
+    <row r="161" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D161" s="10"/>
       <c r="E161" s="21"/>
       <c r="F161" s="10"/>
@@ -21626,7 +21662,7 @@
       <c r="CA161" s="10"/>
       <c r="CB161" s="10"/>
     </row>
-    <row r="162" spans="4:80">
+    <row r="162" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D162" s="10"/>
       <c r="E162" s="21"/>
       <c r="F162" s="10"/>
@@ -21705,7 +21741,7 @@
       <c r="CA162" s="10"/>
       <c r="CB162" s="10"/>
     </row>
-    <row r="163" spans="4:80">
+    <row r="163" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D163" s="10"/>
       <c r="E163" s="21"/>
       <c r="F163" s="10"/>
@@ -21784,7 +21820,7 @@
       <c r="CA163" s="10"/>
       <c r="CB163" s="10"/>
     </row>
-    <row r="164" spans="4:80">
+    <row r="164" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D164" s="10"/>
       <c r="E164" s="21"/>
       <c r="F164" s="10"/>
@@ -21875,7 +21911,7 @@
     <hyperlink ref="A37" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
added sample hl7 template. described here: https://community.hortonworks.com/articles/20318/visualize-patients-complaints-to-their-doctors-usi.html
</commit_message>
<xml_diff>
--- a/NiFi Templates.xlsx
+++ b/NiFi Templates.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vlad\Dropbox\2014 - Hortonworks\Projects\HWX\nifi-templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-102400" yWindow="-15400" windowWidth="36540" windowHeight="20440" tabRatio="500"/>
+    <workbookView xWindow="-102405" yWindow="-15405" windowWidth="36540" windowHeight="20445" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="219">
   <si>
     <t>Template Name:</t>
   </si>
@@ -685,6 +690,12 @@
   </si>
   <si>
     <t>PutElasticsearch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send_HL7_Messages_to_Solr </t>
+  </si>
+  <si>
+    <t>reads HL7 files from a directory, parses the file into segments, and sends to Solr for indexing</t>
   </si>
 </sst>
 </file>
@@ -1137,6 +1148,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1463,536 +1477,536 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ED164"/>
+  <dimension ref="A1:ED163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="CL47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="X45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="EA47" sqref="EA47"/>
+      <selection pane="bottomRight" activeCell="A48" sqref="A48:XFD48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.5" style="8" customWidth="1"/>
-    <col min="3" max="3" width="1.83203125" style="12" customWidth="1"/>
-    <col min="4" max="13" width="4.83203125" customWidth="1"/>
-    <col min="14" max="14" width="1.6640625" style="3" customWidth="1"/>
-    <col min="15" max="133" width="4.83203125" customWidth="1"/>
-    <col min="134" max="134" width="1.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="1.875" style="12" customWidth="1"/>
+    <col min="4" max="13" width="4.875" customWidth="1"/>
+    <col min="14" max="14" width="1.625" style="3" customWidth="1"/>
+    <col min="15" max="133" width="4.875" customWidth="1"/>
+    <col min="134" max="134" width="1.625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:134" ht="16" thickBot="1">
+    <row r="1" spans="1:134" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="26" t="s">
         <v>153</v>
       </c>
       <c r="D1">
-        <f>COUNTIFS(D10:D300,"X")</f>
+        <f>COUNTIFS(D10:D299,"X")</f>
         <v>0</v>
       </c>
       <c r="E1">
-        <f>COUNTIFS(E10:E300,"X")</f>
+        <f>COUNTIFS(E10:E299,"X")</f>
         <v>0</v>
       </c>
       <c r="F1">
-        <f t="shared" ref="F1:M1" si="0">COUNTIFS(F10:F300,"X")</f>
+        <f>COUNTIFS(F10:F299,"X")</f>
         <v>3</v>
       </c>
       <c r="G1">
+        <f>COUNTIFS(G10:G299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="H1">
+        <f>COUNTIFS(H10:H299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="I1">
+        <f>COUNTIFS(I10:I299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="J1">
+        <f>COUNTIFS(J10:J299,"X")</f>
+        <v>2</v>
+      </c>
+      <c r="K1">
+        <f>COUNTIFS(K10:K299,"X")</f>
+        <v>1</v>
+      </c>
+      <c r="L1">
+        <f>COUNTIFS(L10:L299,"X")</f>
+        <v>5</v>
+      </c>
+      <c r="M1">
+        <f>COUNTIFS(M10:M299,"X")</f>
+        <v>2</v>
+      </c>
+      <c r="O1">
+        <f>COUNTIFS(O10:O299,"X")</f>
+        <v>3</v>
+      </c>
+      <c r="P1">
+        <f>COUNTIFS(P10:P299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="Q1">
+        <f>COUNTIFS(Q10:Q299,"X")</f>
+        <v>5</v>
+      </c>
+      <c r="R1">
+        <f>COUNTIFS(R10:R299,"X")</f>
+        <v>1</v>
+      </c>
+      <c r="S1">
+        <f>COUNTIFS(S10:S299,"X")</f>
+        <v>1</v>
+      </c>
+      <c r="T1">
+        <f>COUNTIFS(T10:T299,"X")</f>
+        <v>1</v>
+      </c>
+      <c r="U1">
+        <f>COUNTIFS(U10:U299,"X")</f>
+        <v>2</v>
+      </c>
+      <c r="V1">
+        <f>COUNTIFS(V10:V299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="W1">
+        <f>COUNTIFS(W10:W299,"X")</f>
+        <v>1</v>
+      </c>
+      <c r="X1">
+        <f>COUNTIFS(X10:X299,"X")</f>
+        <v>1</v>
+      </c>
+      <c r="Y1">
+        <f>COUNTIFS(Y10:Y299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="Z1">
+        <f>COUNTIFS(Z10:Z299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="AA1">
+        <f>COUNTIFS(AA10:AA299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="AB1">
+        <f>COUNTIFS(AB10:AB299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="AC1">
+        <f>COUNTIFS(AC10:AC299,"X")</f>
+        <v>3</v>
+      </c>
+      <c r="AD1">
+        <f>COUNTIFS(AD10:AD299,"X")</f>
+        <v>1</v>
+      </c>
+      <c r="AE1">
+        <f>COUNTIFS(AE10:AE299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="AF1">
+        <f>COUNTIFS(AF10:AF299,"X")</f>
+        <v>3</v>
+      </c>
+      <c r="AG1">
+        <f>COUNTIFS(AG10:AG299,"X")</f>
+        <v>8</v>
+      </c>
+      <c r="AH1">
+        <f>COUNTIFS(AH10:AH299,"X")</f>
+        <v>2</v>
+      </c>
+      <c r="AI1">
+        <f>COUNTIFS(AI10:AI299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ1">
+        <f>COUNTIFS(AJ10:AJ299,"X")</f>
+        <v>1</v>
+      </c>
+      <c r="AK1">
+        <f>COUNTIFS(AK10:AK299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="AL1">
+        <f>COUNTIFS(AL10:AL299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="AM1">
+        <f>COUNTIFS(AM10:AM299,"X")</f>
+        <v>3</v>
+      </c>
+      <c r="AN1">
+        <f>COUNTIFS(AN10:AN299,"X")</f>
+        <v>2</v>
+      </c>
+      <c r="AO1">
+        <f>COUNTIFS(AO10:AO299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="AP1">
+        <f>COUNTIFS(AP10:AP299,"X")</f>
+        <v>2</v>
+      </c>
+      <c r="AQ1">
+        <f>COUNTIFS(AQ10:AQ299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="AR1">
+        <f>COUNTIFS(AR10:AR299,"X")</f>
+        <v>1</v>
+      </c>
+      <c r="AS1">
+        <f>COUNTIFS(AS10:AS299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="AT1">
+        <f>COUNTIFS(AT10:AT299,"X")</f>
+        <v>8</v>
+      </c>
+      <c r="AU1">
+        <f>COUNTIFS(AU10:AU299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="AV1">
+        <f>COUNTIFS(AV10:AV299,"X")</f>
+        <v>3</v>
+      </c>
+      <c r="AW1">
+        <f>COUNTIFS(AW10:AW299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="AX1">
+        <f>COUNTIFS(AX10:AX299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="AY1">
+        <f>COUNTIFS(AY10:AY299,"X")</f>
+        <v>1</v>
+      </c>
+      <c r="AZ1">
+        <f>COUNTIFS(AZ10:AZ299,"X")</f>
+        <v>13</v>
+      </c>
+      <c r="BA1">
+        <f>COUNTIFS(BA10:BA299,"X")</f>
+        <v>2</v>
+      </c>
+      <c r="BB1">
+        <f>COUNTIFS(BB10:BB299,"X")</f>
+        <v>9</v>
+      </c>
+      <c r="BC1">
+        <f>COUNTIFS(BC10:BC299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="BD1">
+        <f>COUNTIFS(BD10:BD299,"X")</f>
+        <v>1</v>
+      </c>
+      <c r="BE1">
+        <f>COUNTIFS(BE10:BE299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="BF1">
+        <f>COUNTIFS(BF10:BF299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="BG1">
+        <f>COUNTIFS(BG10:BG299,"X")</f>
+        <v>7</v>
+      </c>
+      <c r="BH1">
+        <f>COUNTIFS(BH10:BH299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="BI1">
+        <f>COUNTIFS(BI10:BI299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="BJ1">
+        <f>COUNTIFS(BJ10:BJ299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="BK1">
+        <f>COUNTIFS(BK10:BK299,"X")</f>
+        <v>1</v>
+      </c>
+      <c r="BL1">
+        <f>COUNTIFS(BL10:BL299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="BM1">
+        <f>COUNTIFS(BM10:BM299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="BN1">
+        <f>COUNTIFS(BN10:BN299,"X")</f>
+        <v>1</v>
+      </c>
+      <c r="BO1">
+        <f>COUNTIFS(BO10:BO299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="BP1">
+        <f>COUNTIFS(BP10:BP299,"X")</f>
+        <v>4</v>
+      </c>
+      <c r="BQ1">
+        <f>COUNTIFS(BQ10:BQ299,"X")</f>
+        <v>5</v>
+      </c>
+      <c r="BR1">
+        <f>COUNTIFS(BR10:BR299,"X")</f>
+        <v>5</v>
+      </c>
+      <c r="BS1">
+        <f>COUNTIFS(BS10:BS299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="BT1">
+        <f>COUNTIFS(BT10:BT299,"X")</f>
+        <v>2</v>
+      </c>
+      <c r="BU1">
+        <f>COUNTIFS(BU10:BU299,"X")</f>
+        <v>3</v>
+      </c>
+      <c r="BV1">
+        <f>COUNTIFS(BV10:BV299,"X")</f>
+        <v>8</v>
+      </c>
+      <c r="BX1">
+        <f>COUNTIFS(BX10:BX299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="BY1">
+        <f>COUNTIFS(BY10:BY299,"X")</f>
+        <v>1</v>
+      </c>
+      <c r="BZ1">
+        <f>COUNTIFS(BZ10:BZ299,"X")</f>
+        <v>2</v>
+      </c>
+      <c r="CA1">
+        <f>COUNTIFS(CA10:CA299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="CB1">
+        <f>COUNTIFS(CB10:CB299,"X")</f>
+        <v>2</v>
+      </c>
+      <c r="CC1">
+        <f>COUNTIFS(CC10:CC299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="CD1">
+        <f>COUNTIFS(CD10:CD299,"X")</f>
+        <v>1</v>
+      </c>
+      <c r="CE1">
+        <f>COUNTIFS(CE10:CE299,"X")</f>
+        <v>11</v>
+      </c>
+      <c r="CF1">
+        <f>COUNTIFS(CF10:CF299,"X")</f>
+        <v>11</v>
+      </c>
+      <c r="CG1">
+        <f>COUNTIFS(CG10:CG299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="CH1">
+        <f>COUNTIFS(CH10:CH299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="CI1">
+        <f>COUNTIFS(CI10:CI299,"X")</f>
+        <v>3</v>
+      </c>
+      <c r="CJ1">
+        <f>COUNTIFS(CJ10:CJ299,"X")</f>
+        <v>1</v>
+      </c>
+      <c r="CK1">
+        <f>COUNTIFS(CK10:CK299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="CM1">
+        <f>COUNTIFS(CM10:CM299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="CN1">
+        <f>COUNTIFS(CN10:CN299,"X")</f>
+        <v>0</v>
+      </c>
+      <c r="CO1">
+        <f>COUNTIFS(CO10:CO299,"X")</f>
+        <v>1</v>
+      </c>
+      <c r="CP1">
+        <f>COUNTIFS(CP10:CP299,"X")</f>
+        <v>2</v>
+      </c>
+      <c r="CQ1">
+        <f t="shared" ref="CQ1:EC1" si="0">COUNTIFS(CQ10:CQ299,"X")</f>
+        <v>13</v>
+      </c>
+      <c r="CR1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H1">
+      <c r="CS1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="CT1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="CU1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="CV1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I1">
+      <c r="CW1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="CX1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="CY1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J1">
+      <c r="CZ1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="DA1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DB1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="DC1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="DD1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DE1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DF1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="DH1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="DI1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="DJ1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DK1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="DL1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="DM1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="K1">
+      <c r="DN1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="DO1">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="L1">
+      <c r="DP1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DQ1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DR1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="DS1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DT1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="DU1">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="M1">
+      <c r="DV1">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="O1">
-        <f>COUNTIFS(O10:O300,"X")</f>
-        <v>2</v>
-      </c>
-      <c r="P1">
-        <f t="shared" ref="P1:CP1" si="1">COUNTIFS(P10:P300,"X")</f>
         <v>0</v>
       </c>
-      <c r="Q1">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="R1">
-        <f t="shared" si="1"/>
+      <c r="DW1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DX1">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="S1">
-        <f t="shared" si="1"/>
+      <c r="DY1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="DZ1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="EA1">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="EB1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="EC1">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="T1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="U1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="V1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="W1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="X1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Z1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AA1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AB1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AC1">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="AD1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AE1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AF1">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="AG1">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="AH1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="AI1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AJ1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AK1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AL1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AM1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="AN1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="AO1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AP1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="AQ1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AR1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AS1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AT1">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="AU1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AV1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="AW1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AX1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AY1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="AZ1">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="BA1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="BB1">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="BC1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="BD1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="BE1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="BF1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="BG1">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="BH1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="BI1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="BJ1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="BK1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="BL1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="BM1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="BN1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="BO1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="BP1">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="BQ1">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="BR1">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="BS1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="BT1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="BU1">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="BV1">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="BX1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="BY1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="BZ1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="CA1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="CB1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="CC1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="CD1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="CE1">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="CF1">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="CG1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="CH1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="CI1">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="CJ1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="CK1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="CM1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="CN1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="CO1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="CP1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="CQ1">
-        <f t="shared" ref="CQ1:EC1" si="2">COUNTIFS(CQ10:CQ300,"X")</f>
-        <v>13</v>
-      </c>
-      <c r="CR1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="CS1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="CT1">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="CU1">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="CV1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="CW1">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="CX1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="CY1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="CZ1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="DA1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="DB1">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="DC1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="DD1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="DE1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="DF1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="DH1">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="DI1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="DJ1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="DK1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="DL1">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-      <c r="DM1">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="DN1">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="DO1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="DP1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="DQ1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="DR1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="DS1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="DT1">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="DU1">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="DV1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="DW1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="DX1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="DY1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="DZ1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="EA1">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="EB1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="EC1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:134" s="5" customFormat="1" ht="48" customHeight="1" thickBot="1">
+    <row r="2" spans="1:134" s="5" customFormat="1" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="29" t="s">
         <v>183</v>
       </c>
@@ -2134,7 +2148,7 @@
       <c r="EC2" s="32"/>
       <c r="ED2" s="6"/>
     </row>
-    <row r="3" spans="1:134" s="1" customFormat="1" ht="221" customHeight="1" thickTop="1">
+    <row r="3" spans="1:134" s="1" customFormat="1" ht="221.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30"/>
       <c r="B3" s="30"/>
       <c r="C3" s="20"/>
@@ -2528,11 +2542,11 @@
       </c>
       <c r="ED3" s="4"/>
     </row>
-    <row r="4" spans="1:134" s="3" customFormat="1" ht="8" customHeight="1">
+    <row r="4" spans="1:134" s="3" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
       <c r="C4" s="12"/>
     </row>
-    <row r="5" spans="1:134">
+    <row r="5" spans="1:134" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>25</v>
       </c>
@@ -2620,7 +2634,7 @@
       <c r="CA5" s="10"/>
       <c r="CB5" s="10"/>
     </row>
-    <row r="6" spans="1:134">
+    <row r="6" spans="1:134" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>26</v>
       </c>
@@ -2714,7 +2728,7 @@
       <c r="CA6" s="10"/>
       <c r="CB6" s="10"/>
     </row>
-    <row r="7" spans="1:134">
+    <row r="7" spans="1:134" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>28</v>
       </c>
@@ -2808,7 +2822,7 @@
       <c r="CA7" s="10"/>
       <c r="CB7" s="10"/>
     </row>
-    <row r="8" spans="1:134" s="3" customFormat="1" ht="7" customHeight="1" thickBot="1">
+    <row r="8" spans="1:134" s="3" customFormat="1" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
       <c r="C8" s="12"/>
       <c r="D8" s="11"/>
@@ -2889,7 +2903,7 @@
       <c r="CA8" s="11"/>
       <c r="CB8" s="11"/>
     </row>
-    <row r="9" spans="1:134" ht="25" customHeight="1" thickTop="1">
+    <row r="9" spans="1:134" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>0</v>
       </c>
@@ -3027,7 +3041,7 @@
       <c r="EB9" s="34"/>
       <c r="EC9" s="34"/>
     </row>
-    <row r="10" spans="1:134" ht="120">
+    <row r="10" spans="1:134" ht="126" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>110</v>
       </c>
@@ -3201,7 +3215,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:134" ht="90">
+    <row r="11" spans="1:134" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>111</v>
       </c>
@@ -3351,7 +3365,7 @@
       <c r="EB11" s="13"/>
       <c r="EC11" s="13"/>
     </row>
-    <row r="12" spans="1:134" ht="72" customHeight="1">
+    <row r="12" spans="1:134" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>112</v>
       </c>
@@ -3497,7 +3511,7 @@
       <c r="EB12" s="13"/>
       <c r="EC12" s="13"/>
     </row>
-    <row r="13" spans="1:134" ht="72" customHeight="1">
+    <row r="13" spans="1:134" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>115</v>
       </c>
@@ -3645,7 +3659,7 @@
       <c r="EB13" s="13"/>
       <c r="EC13" s="13"/>
     </row>
-    <row r="14" spans="1:134" ht="90">
+    <row r="14" spans="1:134" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>116</v>
       </c>
@@ -3789,7 +3803,7 @@
       <c r="EB14" s="13"/>
       <c r="EC14" s="13"/>
     </row>
-    <row r="15" spans="1:134" ht="90">
+    <row r="15" spans="1:134" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>119</v>
       </c>
@@ -3943,7 +3957,7 @@
       <c r="EB15" s="13"/>
       <c r="EC15" s="13"/>
     </row>
-    <row r="16" spans="1:134" ht="72" customHeight="1">
+    <row r="16" spans="1:134" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>122</v>
       </c>
@@ -4093,7 +4107,7 @@
       <c r="EB16" s="13"/>
       <c r="EC16" s="13"/>
     </row>
-    <row r="17" spans="1:133" ht="120">
+    <row r="17" spans="1:133" ht="126" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>123</v>
       </c>
@@ -4241,7 +4255,7 @@
       <c r="EB17" s="13"/>
       <c r="EC17" s="13"/>
     </row>
-    <row r="18" spans="1:133" ht="72" customHeight="1">
+    <row r="18" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>126</v>
       </c>
@@ -4405,7 +4419,7 @@
       <c r="EB18" s="13"/>
       <c r="EC18" s="13"/>
     </row>
-    <row r="19" spans="1:133" ht="72" customHeight="1">
+    <row r="19" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>127</v>
       </c>
@@ -4549,7 +4563,7 @@
       <c r="EB19" s="13"/>
       <c r="EC19" s="13"/>
     </row>
-    <row r="20" spans="1:133" ht="90">
+    <row r="20" spans="1:133" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>128</v>
       </c>
@@ -4691,7 +4705,7 @@
       <c r="EB20" s="13"/>
       <c r="EC20" s="13"/>
     </row>
-    <row r="21" spans="1:133" ht="72" customHeight="1">
+    <row r="21" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>131</v>
       </c>
@@ -4837,7 +4851,7 @@
       <c r="EB21" s="13"/>
       <c r="EC21" s="13"/>
     </row>
-    <row r="22" spans="1:133" ht="105">
+    <row r="22" spans="1:133" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>133</v>
       </c>
@@ -4987,7 +5001,7 @@
       <c r="EB22" s="13"/>
       <c r="EC22" s="13"/>
     </row>
-    <row r="23" spans="1:133" ht="105">
+    <row r="23" spans="1:133" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>136</v>
       </c>
@@ -5135,7 +5149,7 @@
       <c r="EB23" s="13"/>
       <c r="EC23" s="13"/>
     </row>
-    <row r="24" spans="1:133" ht="120">
+    <row r="24" spans="1:133" ht="126" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>138</v>
       </c>
@@ -5279,7 +5293,7 @@
       <c r="EB24" s="13"/>
       <c r="EC24" s="13"/>
     </row>
-    <row r="25" spans="1:133" ht="75">
+    <row r="25" spans="1:133" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>140</v>
       </c>
@@ -5425,7 +5439,7 @@
       <c r="EB25" s="13"/>
       <c r="EC25" s="13"/>
     </row>
-    <row r="26" spans="1:133" ht="240">
+    <row r="26" spans="1:133" ht="283.5" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>142</v>
       </c>
@@ -5577,7 +5591,7 @@
       <c r="EB26" s="13"/>
       <c r="EC26" s="13"/>
     </row>
-    <row r="27" spans="1:133" ht="330">
+    <row r="27" spans="1:133" ht="346.5" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>144</v>
       </c>
@@ -5723,7 +5737,7 @@
       <c r="EB27" s="13"/>
       <c r="EC27" s="13"/>
     </row>
-    <row r="28" spans="1:133" ht="409">
+    <row r="28" spans="1:133" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>147</v>
       </c>
@@ -5881,7 +5895,7 @@
       <c r="EB28" s="13"/>
       <c r="EC28" s="13"/>
     </row>
-    <row r="29" spans="1:133" ht="72" customHeight="1">
+    <row r="29" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>163</v>
       </c>
@@ -6029,7 +6043,7 @@
       <c r="EB29" s="13"/>
       <c r="EC29" s="13"/>
     </row>
-    <row r="30" spans="1:133" ht="105">
+    <row r="30" spans="1:133" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>165</v>
       </c>
@@ -6183,7 +6197,7 @@
       <c r="EB30" s="13"/>
       <c r="EC30" s="13"/>
     </row>
-    <row r="31" spans="1:133" ht="165">
+    <row r="31" spans="1:133" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>168</v>
       </c>
@@ -6353,7 +6367,7 @@
       <c r="EB31" s="13"/>
       <c r="EC31" s="13"/>
     </row>
-    <row r="32" spans="1:133" ht="72" customHeight="1">
+    <row r="32" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>169</v>
       </c>
@@ -6501,7 +6515,7 @@
       <c r="EB32" s="13"/>
       <c r="EC32" s="13"/>
     </row>
-    <row r="33" spans="1:133" ht="72" customHeight="1">
+    <row r="33" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
         <v>171</v>
       </c>
@@ -6647,7 +6661,7 @@
       <c r="EB33" s="13"/>
       <c r="EC33" s="13"/>
     </row>
-    <row r="34" spans="1:133" ht="72" customHeight="1">
+    <row r="34" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>173</v>
       </c>
@@ -6801,7 +6815,7 @@
       <c r="EB34" s="13"/>
       <c r="EC34" s="13"/>
     </row>
-    <row r="35" spans="1:133" ht="72" customHeight="1">
+    <row r="35" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>175</v>
       </c>
@@ -6969,7 +6983,7 @@
       <c r="EB35" s="13"/>
       <c r="EC35" s="13"/>
     </row>
-    <row r="36" spans="1:133" ht="72" customHeight="1">
+    <row r="36" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>178</v>
       </c>
@@ -7123,7 +7137,7 @@
       <c r="EB36" s="13"/>
       <c r="EC36" s="13"/>
     </row>
-    <row r="37" spans="1:133" ht="72" customHeight="1">
+    <row r="37" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>179</v>
       </c>
@@ -7281,7 +7295,7 @@
       <c r="EB37" s="13"/>
       <c r="EC37" s="13"/>
     </row>
-    <row r="38" spans="1:133" ht="72" customHeight="1">
+    <row r="38" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
         <v>184</v>
       </c>
@@ -7429,7 +7443,7 @@
       <c r="EB38" s="13"/>
       <c r="EC38" s="13"/>
     </row>
-    <row r="39" spans="1:133" ht="72" customHeight="1">
+    <row r="39" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>186</v>
       </c>
@@ -7577,7 +7591,7 @@
       <c r="EB39" s="13"/>
       <c r="EC39" s="13"/>
     </row>
-    <row r="40" spans="1:133" ht="72" customHeight="1">
+    <row r="40" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>190</v>
       </c>
@@ -7743,7 +7757,7 @@
       <c r="EB40" s="13"/>
       <c r="EC40" s="13"/>
     </row>
-    <row r="41" spans="1:133" ht="72" customHeight="1">
+    <row r="41" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>193</v>
       </c>
@@ -7895,7 +7909,7 @@
       <c r="EB41" s="13"/>
       <c r="EC41" s="13"/>
     </row>
-    <row r="42" spans="1:133" ht="72" customHeight="1">
+    <row r="42" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>195</v>
       </c>
@@ -8047,7 +8061,7 @@
       <c r="EB42" s="13"/>
       <c r="EC42" s="13"/>
     </row>
-    <row r="43" spans="1:133" ht="72" customHeight="1">
+    <row r="43" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>197</v>
       </c>
@@ -8193,7 +8207,7 @@
       <c r="EB43" s="13"/>
       <c r="EC43" s="13"/>
     </row>
-    <row r="44" spans="1:133" ht="72" customHeight="1">
+    <row r="44" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>199</v>
       </c>
@@ -8341,7 +8355,7 @@
       <c r="EB44" s="13"/>
       <c r="EC44" s="13"/>
     </row>
-    <row r="45" spans="1:133" ht="72" customHeight="1">
+    <row r="45" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>204</v>
       </c>
@@ -8497,7 +8511,7 @@
       <c r="EB45" s="13"/>
       <c r="EC45" s="13"/>
     </row>
-    <row r="46" spans="1:133" ht="72" customHeight="1">
+    <row r="46" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>209</v>
       </c>
@@ -8645,7 +8659,7 @@
       <c r="EB46" s="13"/>
       <c r="EC46" s="13"/>
     </row>
-    <row r="47" spans="1:133" ht="72" customHeight="1">
+    <row r="47" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>213</v>
       </c>
@@ -8803,9 +8817,13 @@
       <c r="EB47" s="13"/>
       <c r="EC47" s="13"/>
     </row>
-    <row r="48" spans="1:133" ht="72" customHeight="1">
-      <c r="A48" s="16"/>
-      <c r="B48" s="24"/>
+    <row r="48" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>218</v>
+      </c>
       <c r="D48" s="18"/>
       <c r="E48" s="18"/>
       <c r="F48" s="13"/>
@@ -8817,7 +8835,9 @@
       <c r="L48" s="13"/>
       <c r="M48" s="13"/>
       <c r="N48" s="14"/>
-      <c r="O48" s="13"/>
+      <c r="O48" s="13" t="s">
+        <v>191</v>
+      </c>
       <c r="P48" s="13"/>
       <c r="Q48" s="13"/>
       <c r="R48" s="13"/>
@@ -8841,16 +8861,22 @@
       <c r="AJ48" s="13"/>
       <c r="AK48" s="13"/>
       <c r="AL48" s="13"/>
-      <c r="AM48" s="13"/>
+      <c r="AM48" s="13" t="s">
+        <v>191</v>
+      </c>
       <c r="AN48" s="13"/>
       <c r="AO48" s="13"/>
       <c r="AP48" s="13"/>
       <c r="AQ48" s="13"/>
-      <c r="AR48" s="13"/>
+      <c r="AR48" s="13" t="s">
+        <v>191</v>
+      </c>
       <c r="AS48" s="13"/>
       <c r="AT48" s="13"/>
       <c r="AU48" s="13"/>
-      <c r="AV48" s="13"/>
+      <c r="AV48" s="13" t="s">
+        <v>191</v>
+      </c>
       <c r="AW48" s="13"/>
       <c r="AX48" s="13"/>
       <c r="AY48" s="13"/>
@@ -8908,7 +8934,9 @@
       <c r="CY48" s="13"/>
       <c r="CZ48" s="13"/>
       <c r="DA48" s="13"/>
-      <c r="DB48" s="13"/>
+      <c r="DB48" s="13" t="s">
+        <v>191</v>
+      </c>
       <c r="DC48" s="13"/>
       <c r="DD48" s="13"/>
       <c r="DE48" s="13"/>
@@ -8933,11 +8961,13 @@
       <c r="DX48" s="13"/>
       <c r="DY48" s="13"/>
       <c r="DZ48" s="13"/>
-      <c r="EA48" s="13"/>
+      <c r="EA48" s="13" t="s">
+        <v>191</v>
+      </c>
       <c r="EB48" s="13"/>
       <c r="EC48" s="13"/>
     </row>
-    <row r="49" spans="1:133" ht="72" customHeight="1">
+    <row r="49" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16"/>
       <c r="B49" s="24"/>
       <c r="D49" s="18"/>
@@ -9071,7 +9101,7 @@
       <c r="EB49" s="13"/>
       <c r="EC49" s="13"/>
     </row>
-    <row r="50" spans="1:133" ht="72" customHeight="1">
+    <row r="50" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="16"/>
       <c r="B50" s="24"/>
       <c r="D50" s="18"/>
@@ -9205,7 +9235,7 @@
       <c r="EB50" s="13"/>
       <c r="EC50" s="13"/>
     </row>
-    <row r="51" spans="1:133" ht="72" customHeight="1">
+    <row r="51" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16"/>
       <c r="B51" s="24"/>
       <c r="D51" s="18"/>
@@ -9339,7 +9369,7 @@
       <c r="EB51" s="13"/>
       <c r="EC51" s="13"/>
     </row>
-    <row r="52" spans="1:133" ht="72" customHeight="1">
+    <row r="52" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="16"/>
       <c r="B52" s="24"/>
       <c r="D52" s="18"/>
@@ -9473,7 +9503,7 @@
       <c r="EB52" s="13"/>
       <c r="EC52" s="13"/>
     </row>
-    <row r="53" spans="1:133" ht="72" customHeight="1">
+    <row r="53" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16"/>
       <c r="B53" s="24"/>
       <c r="D53" s="18"/>
@@ -9607,7 +9637,7 @@
       <c r="EB53" s="13"/>
       <c r="EC53" s="13"/>
     </row>
-    <row r="54" spans="1:133" ht="72" customHeight="1">
+    <row r="54" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="16"/>
       <c r="B54" s="24"/>
       <c r="D54" s="18"/>
@@ -9741,7 +9771,7 @@
       <c r="EB54" s="13"/>
       <c r="EC54" s="13"/>
     </row>
-    <row r="55" spans="1:133" ht="72" customHeight="1">
+    <row r="55" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="16"/>
       <c r="B55" s="24"/>
       <c r="D55" s="18"/>
@@ -9875,7 +9905,7 @@
       <c r="EB55" s="13"/>
       <c r="EC55" s="13"/>
     </row>
-    <row r="56" spans="1:133" ht="72" customHeight="1">
+    <row r="56" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="16"/>
       <c r="B56" s="24"/>
       <c r="D56" s="18"/>
@@ -10009,7 +10039,7 @@
       <c r="EB56" s="13"/>
       <c r="EC56" s="13"/>
     </row>
-    <row r="57" spans="1:133" ht="72" customHeight="1">
+    <row r="57" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16"/>
       <c r="B57" s="24"/>
       <c r="D57" s="18"/>
@@ -10143,7 +10173,7 @@
       <c r="EB57" s="13"/>
       <c r="EC57" s="13"/>
     </row>
-    <row r="58" spans="1:133" ht="72" customHeight="1">
+    <row r="58" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="16"/>
       <c r="B58" s="24"/>
       <c r="D58" s="18"/>
@@ -10277,7 +10307,7 @@
       <c r="EB58" s="13"/>
       <c r="EC58" s="13"/>
     </row>
-    <row r="59" spans="1:133" ht="72" customHeight="1">
+    <row r="59" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="16"/>
       <c r="B59" s="24"/>
       <c r="D59" s="18"/>
@@ -10411,7 +10441,7 @@
       <c r="EB59" s="13"/>
       <c r="EC59" s="13"/>
     </row>
-    <row r="60" spans="1:133" ht="72" customHeight="1">
+    <row r="60" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="16"/>
       <c r="B60" s="24"/>
       <c r="D60" s="18"/>
@@ -10545,7 +10575,7 @@
       <c r="EB60" s="13"/>
       <c r="EC60" s="13"/>
     </row>
-    <row r="61" spans="1:133" ht="72" customHeight="1">
+    <row r="61" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="16"/>
       <c r="B61" s="24"/>
       <c r="D61" s="18"/>
@@ -10679,7 +10709,7 @@
       <c r="EB61" s="13"/>
       <c r="EC61" s="13"/>
     </row>
-    <row r="62" spans="1:133" ht="72" customHeight="1">
+    <row r="62" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="16"/>
       <c r="B62" s="24"/>
       <c r="D62" s="18"/>
@@ -10813,7 +10843,7 @@
       <c r="EB62" s="13"/>
       <c r="EC62" s="13"/>
     </row>
-    <row r="63" spans="1:133" ht="72" customHeight="1">
+    <row r="63" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="16"/>
       <c r="B63" s="24"/>
       <c r="D63" s="18"/>
@@ -10947,7 +10977,7 @@
       <c r="EB63" s="13"/>
       <c r="EC63" s="13"/>
     </row>
-    <row r="64" spans="1:133" ht="72" customHeight="1">
+    <row r="64" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="16"/>
       <c r="B64" s="24"/>
       <c r="D64" s="18"/>
@@ -11081,7 +11111,7 @@
       <c r="EB64" s="13"/>
       <c r="EC64" s="13"/>
     </row>
-    <row r="65" spans="1:133" ht="72" customHeight="1">
+    <row r="65" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="16"/>
       <c r="B65" s="24"/>
       <c r="D65" s="18"/>
@@ -11215,7 +11245,7 @@
       <c r="EB65" s="13"/>
       <c r="EC65" s="13"/>
     </row>
-    <row r="66" spans="1:133" ht="72" customHeight="1">
+    <row r="66" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="16"/>
       <c r="B66" s="24"/>
       <c r="D66" s="18"/>
@@ -11349,7 +11379,7 @@
       <c r="EB66" s="13"/>
       <c r="EC66" s="13"/>
     </row>
-    <row r="67" spans="1:133" ht="72" customHeight="1">
+    <row r="67" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="16"/>
       <c r="B67" s="24"/>
       <c r="D67" s="18"/>
@@ -11483,7 +11513,7 @@
       <c r="EB67" s="13"/>
       <c r="EC67" s="13"/>
     </row>
-    <row r="68" spans="1:133" ht="72" customHeight="1">
+    <row r="68" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="16"/>
       <c r="B68" s="24"/>
       <c r="D68" s="18"/>
@@ -11617,7 +11647,7 @@
       <c r="EB68" s="13"/>
       <c r="EC68" s="13"/>
     </row>
-    <row r="69" spans="1:133" ht="72" customHeight="1">
+    <row r="69" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="16"/>
       <c r="B69" s="24"/>
       <c r="D69" s="18"/>
@@ -11751,7 +11781,7 @@
       <c r="EB69" s="13"/>
       <c r="EC69" s="13"/>
     </row>
-    <row r="70" spans="1:133" ht="72" customHeight="1">
+    <row r="70" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="16"/>
       <c r="B70" s="24"/>
       <c r="D70" s="18"/>
@@ -11885,7 +11915,7 @@
       <c r="EB70" s="13"/>
       <c r="EC70" s="13"/>
     </row>
-    <row r="71" spans="1:133" ht="72" customHeight="1">
+    <row r="71" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="16"/>
       <c r="B71" s="24"/>
       <c r="D71" s="18"/>
@@ -12019,7 +12049,7 @@
       <c r="EB71" s="13"/>
       <c r="EC71" s="13"/>
     </row>
-    <row r="72" spans="1:133" ht="72" customHeight="1">
+    <row r="72" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="16"/>
       <c r="B72" s="24"/>
       <c r="D72" s="18"/>
@@ -12153,7 +12183,7 @@
       <c r="EB72" s="13"/>
       <c r="EC72" s="13"/>
     </row>
-    <row r="73" spans="1:133" ht="72" customHeight="1">
+    <row r="73" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="16"/>
       <c r="B73" s="24"/>
       <c r="D73" s="18"/>
@@ -12287,7 +12317,7 @@
       <c r="EB73" s="13"/>
       <c r="EC73" s="13"/>
     </row>
-    <row r="74" spans="1:133" ht="72" customHeight="1">
+    <row r="74" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="16"/>
       <c r="B74" s="24"/>
       <c r="D74" s="18"/>
@@ -12421,7 +12451,7 @@
       <c r="EB74" s="13"/>
       <c r="EC74" s="13"/>
     </row>
-    <row r="75" spans="1:133" ht="72" customHeight="1">
+    <row r="75" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="16"/>
       <c r="B75" s="24"/>
       <c r="D75" s="18"/>
@@ -12555,7 +12585,7 @@
       <c r="EB75" s="13"/>
       <c r="EC75" s="13"/>
     </row>
-    <row r="76" spans="1:133" ht="72" customHeight="1">
+    <row r="76" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="16"/>
       <c r="B76" s="24"/>
       <c r="D76" s="18"/>
@@ -12689,7 +12719,7 @@
       <c r="EB76" s="13"/>
       <c r="EC76" s="13"/>
     </row>
-    <row r="77" spans="1:133" ht="72" customHeight="1">
+    <row r="77" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="16"/>
       <c r="B77" s="24"/>
       <c r="D77" s="18"/>
@@ -12823,7 +12853,7 @@
       <c r="EB77" s="13"/>
       <c r="EC77" s="13"/>
     </row>
-    <row r="78" spans="1:133" ht="72" customHeight="1">
+    <row r="78" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="16"/>
       <c r="B78" s="24"/>
       <c r="D78" s="18"/>
@@ -12957,7 +12987,7 @@
       <c r="EB78" s="13"/>
       <c r="EC78" s="13"/>
     </row>
-    <row r="79" spans="1:133" ht="72" customHeight="1">
+    <row r="79" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="16"/>
       <c r="B79" s="24"/>
       <c r="D79" s="18"/>
@@ -13091,7 +13121,7 @@
       <c r="EB79" s="13"/>
       <c r="EC79" s="13"/>
     </row>
-    <row r="80" spans="1:133" ht="72" customHeight="1">
+    <row r="80" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="16"/>
       <c r="B80" s="24"/>
       <c r="D80" s="18"/>
@@ -13225,7 +13255,7 @@
       <c r="EB80" s="13"/>
       <c r="EC80" s="13"/>
     </row>
-    <row r="81" spans="1:133" ht="72" customHeight="1">
+    <row r="81" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="16"/>
       <c r="B81" s="24"/>
       <c r="D81" s="18"/>
@@ -13359,7 +13389,7 @@
       <c r="EB81" s="13"/>
       <c r="EC81" s="13"/>
     </row>
-    <row r="82" spans="1:133" ht="72" customHeight="1">
+    <row r="82" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="16"/>
       <c r="B82" s="24"/>
       <c r="D82" s="18"/>
@@ -13493,7 +13523,7 @@
       <c r="EB82" s="13"/>
       <c r="EC82" s="13"/>
     </row>
-    <row r="83" spans="1:133" ht="72" customHeight="1">
+    <row r="83" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="16"/>
       <c r="B83" s="24"/>
       <c r="D83" s="18"/>
@@ -13627,7 +13657,7 @@
       <c r="EB83" s="13"/>
       <c r="EC83" s="13"/>
     </row>
-    <row r="84" spans="1:133" ht="72" customHeight="1">
+    <row r="84" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="16"/>
       <c r="B84" s="24"/>
       <c r="D84" s="18"/>
@@ -13761,7 +13791,7 @@
       <c r="EB84" s="13"/>
       <c r="EC84" s="13"/>
     </row>
-    <row r="85" spans="1:133" ht="72" customHeight="1">
+    <row r="85" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="16"/>
       <c r="B85" s="24"/>
       <c r="D85" s="18"/>
@@ -13895,7 +13925,7 @@
       <c r="EB85" s="13"/>
       <c r="EC85" s="13"/>
     </row>
-    <row r="86" spans="1:133" ht="72" customHeight="1">
+    <row r="86" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="16"/>
       <c r="B86" s="24"/>
       <c r="D86" s="18"/>
@@ -14029,7 +14059,7 @@
       <c r="EB86" s="13"/>
       <c r="EC86" s="13"/>
     </row>
-    <row r="87" spans="1:133" ht="72" customHeight="1">
+    <row r="87" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="16"/>
       <c r="B87" s="24"/>
       <c r="D87" s="18"/>
@@ -14163,7 +14193,7 @@
       <c r="EB87" s="13"/>
       <c r="EC87" s="13"/>
     </row>
-    <row r="88" spans="1:133" ht="72" customHeight="1">
+    <row r="88" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="16"/>
       <c r="B88" s="24"/>
       <c r="D88" s="18"/>
@@ -14297,7 +14327,7 @@
       <c r="EB88" s="13"/>
       <c r="EC88" s="13"/>
     </row>
-    <row r="89" spans="1:133" ht="72" customHeight="1">
+    <row r="89" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="16"/>
       <c r="B89" s="24"/>
       <c r="D89" s="18"/>
@@ -14431,7 +14461,7 @@
       <c r="EB89" s="13"/>
       <c r="EC89" s="13"/>
     </row>
-    <row r="90" spans="1:133" ht="72" customHeight="1">
+    <row r="90" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="16"/>
       <c r="B90" s="24"/>
       <c r="D90" s="18"/>
@@ -14565,7 +14595,7 @@
       <c r="EB90" s="13"/>
       <c r="EC90" s="13"/>
     </row>
-    <row r="91" spans="1:133" ht="72" customHeight="1">
+    <row r="91" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="16"/>
       <c r="B91" s="24"/>
       <c r="D91" s="18"/>
@@ -14699,7 +14729,7 @@
       <c r="EB91" s="13"/>
       <c r="EC91" s="13"/>
     </row>
-    <row r="92" spans="1:133" ht="72" customHeight="1">
+    <row r="92" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="16"/>
       <c r="B92" s="24"/>
       <c r="D92" s="18"/>
@@ -14833,7 +14863,7 @@
       <c r="EB92" s="13"/>
       <c r="EC92" s="13"/>
     </row>
-    <row r="93" spans="1:133" ht="72" customHeight="1">
+    <row r="93" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="16"/>
       <c r="B93" s="24"/>
       <c r="D93" s="18"/>
@@ -14967,7 +14997,7 @@
       <c r="EB93" s="13"/>
       <c r="EC93" s="13"/>
     </row>
-    <row r="94" spans="1:133" ht="72" customHeight="1">
+    <row r="94" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="16"/>
       <c r="B94" s="24"/>
       <c r="D94" s="18"/>
@@ -15101,7 +15131,7 @@
       <c r="EB94" s="13"/>
       <c r="EC94" s="13"/>
     </row>
-    <row r="95" spans="1:133" ht="72" customHeight="1">
+    <row r="95" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="16"/>
       <c r="B95" s="24"/>
       <c r="D95" s="18"/>
@@ -15235,7 +15265,7 @@
       <c r="EB95" s="13"/>
       <c r="EC95" s="13"/>
     </row>
-    <row r="96" spans="1:133" ht="72" customHeight="1">
+    <row r="96" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="16"/>
       <c r="B96" s="24"/>
       <c r="D96" s="18"/>
@@ -15369,7 +15399,7 @@
       <c r="EB96" s="13"/>
       <c r="EC96" s="13"/>
     </row>
-    <row r="97" spans="1:133" ht="72" customHeight="1">
+    <row r="97" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="16"/>
       <c r="B97" s="24"/>
       <c r="D97" s="18"/>
@@ -15503,7 +15533,7 @@
       <c r="EB97" s="13"/>
       <c r="EC97" s="13"/>
     </row>
-    <row r="98" spans="1:133" ht="72" customHeight="1">
+    <row r="98" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="16"/>
       <c r="B98" s="24"/>
       <c r="D98" s="18"/>
@@ -15637,7 +15667,7 @@
       <c r="EB98" s="13"/>
       <c r="EC98" s="13"/>
     </row>
-    <row r="99" spans="1:133" ht="72" customHeight="1">
+    <row r="99" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="16"/>
       <c r="B99" s="24"/>
       <c r="D99" s="18"/>
@@ -15771,7 +15801,7 @@
       <c r="EB99" s="13"/>
       <c r="EC99" s="13"/>
     </row>
-    <row r="100" spans="1:133" ht="72" customHeight="1">
+    <row r="100" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="16"/>
       <c r="B100" s="24"/>
       <c r="D100" s="18"/>
@@ -15905,7 +15935,7 @@
       <c r="EB100" s="13"/>
       <c r="EC100" s="13"/>
     </row>
-    <row r="101" spans="1:133" ht="72" customHeight="1">
+    <row r="101" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="16"/>
       <c r="B101" s="24"/>
       <c r="D101" s="18"/>
@@ -16039,7 +16069,7 @@
       <c r="EB101" s="13"/>
       <c r="EC101" s="13"/>
     </row>
-    <row r="102" spans="1:133" ht="72" customHeight="1">
+    <row r="102" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="16"/>
       <c r="B102" s="24"/>
       <c r="D102" s="18"/>
@@ -16173,7 +16203,7 @@
       <c r="EB102" s="13"/>
       <c r="EC102" s="13"/>
     </row>
-    <row r="103" spans="1:133" ht="72" customHeight="1">
+    <row r="103" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="16"/>
       <c r="B103" s="24"/>
       <c r="D103" s="18"/>
@@ -16307,7 +16337,7 @@
       <c r="EB103" s="13"/>
       <c r="EC103" s="13"/>
     </row>
-    <row r="104" spans="1:133" ht="72" customHeight="1">
+    <row r="104" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="16"/>
       <c r="B104" s="24"/>
       <c r="D104" s="18"/>
@@ -16441,7 +16471,7 @@
       <c r="EB104" s="13"/>
       <c r="EC104" s="13"/>
     </row>
-    <row r="105" spans="1:133" ht="72" customHeight="1">
+    <row r="105" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="16"/>
       <c r="B105" s="24"/>
       <c r="D105" s="18"/>
@@ -16575,7 +16605,7 @@
       <c r="EB105" s="13"/>
       <c r="EC105" s="13"/>
     </row>
-    <row r="106" spans="1:133" ht="72" customHeight="1">
+    <row r="106" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="16"/>
       <c r="B106" s="24"/>
       <c r="D106" s="18"/>
@@ -16709,7 +16739,7 @@
       <c r="EB106" s="13"/>
       <c r="EC106" s="13"/>
     </row>
-    <row r="107" spans="1:133" ht="72" customHeight="1">
+    <row r="107" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="16"/>
       <c r="B107" s="24"/>
       <c r="D107" s="18"/>
@@ -16843,7 +16873,7 @@
       <c r="EB107" s="13"/>
       <c r="EC107" s="13"/>
     </row>
-    <row r="108" spans="1:133" ht="72" customHeight="1">
+    <row r="108" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="16"/>
       <c r="B108" s="24"/>
       <c r="D108" s="18"/>
@@ -16977,7 +17007,7 @@
       <c r="EB108" s="13"/>
       <c r="EC108" s="13"/>
     </row>
-    <row r="109" spans="1:133" ht="72" customHeight="1">
+    <row r="109" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="16"/>
       <c r="B109" s="24"/>
       <c r="D109" s="18"/>
@@ -17111,7 +17141,7 @@
       <c r="EB109" s="13"/>
       <c r="EC109" s="13"/>
     </row>
-    <row r="110" spans="1:133" ht="72" customHeight="1">
+    <row r="110" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="16"/>
       <c r="B110" s="24"/>
       <c r="D110" s="18"/>
@@ -17245,7 +17275,7 @@
       <c r="EB110" s="13"/>
       <c r="EC110" s="13"/>
     </row>
-    <row r="111" spans="1:133" ht="72" customHeight="1">
+    <row r="111" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="16"/>
       <c r="B111" s="24"/>
       <c r="D111" s="18"/>
@@ -17379,7 +17409,7 @@
       <c r="EB111" s="13"/>
       <c r="EC111" s="13"/>
     </row>
-    <row r="112" spans="1:133" ht="72" customHeight="1">
+    <row r="112" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="16"/>
       <c r="B112" s="24"/>
       <c r="D112" s="18"/>
@@ -17513,7 +17543,7 @@
       <c r="EB112" s="13"/>
       <c r="EC112" s="13"/>
     </row>
-    <row r="113" spans="1:133" ht="72" customHeight="1">
+    <row r="113" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="16"/>
       <c r="B113" s="24"/>
       <c r="D113" s="18"/>
@@ -17647,7 +17677,7 @@
       <c r="EB113" s="13"/>
       <c r="EC113" s="13"/>
     </row>
-    <row r="114" spans="1:133" ht="72" customHeight="1">
+    <row r="114" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="16"/>
       <c r="B114" s="24"/>
       <c r="D114" s="18"/>
@@ -17781,7 +17811,7 @@
       <c r="EB114" s="13"/>
       <c r="EC114" s="13"/>
     </row>
-    <row r="115" spans="1:133" ht="72" customHeight="1">
+    <row r="115" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="16"/>
       <c r="B115" s="24"/>
       <c r="D115" s="18"/>
@@ -17915,141 +17945,87 @@
       <c r="EB115" s="13"/>
       <c r="EC115" s="13"/>
     </row>
-    <row r="116" spans="1:133" ht="72" customHeight="1">
-      <c r="A116" s="16"/>
-      <c r="B116" s="24"/>
-      <c r="D116" s="18"/>
-      <c r="E116" s="18"/>
-      <c r="F116" s="13"/>
-      <c r="G116" s="13"/>
-      <c r="H116" s="13"/>
-      <c r="I116" s="13"/>
-      <c r="J116" s="13"/>
-      <c r="K116" s="13"/>
-      <c r="L116" s="13"/>
-      <c r="M116" s="13"/>
-      <c r="N116" s="14"/>
-      <c r="O116" s="13"/>
-      <c r="P116" s="13"/>
-      <c r="Q116" s="13"/>
-      <c r="R116" s="13"/>
-      <c r="S116" s="13"/>
-      <c r="T116" s="13"/>
-      <c r="U116" s="13"/>
-      <c r="V116" s="13"/>
-      <c r="W116" s="13"/>
-      <c r="X116" s="13"/>
-      <c r="Y116" s="13"/>
-      <c r="Z116" s="13"/>
-      <c r="AA116" s="13"/>
-      <c r="AB116" s="13"/>
-      <c r="AC116" s="13"/>
-      <c r="AD116" s="13"/>
-      <c r="AE116" s="13"/>
-      <c r="AF116" s="13"/>
-      <c r="AG116" s="13"/>
-      <c r="AH116" s="13"/>
-      <c r="AI116" s="13"/>
-      <c r="AJ116" s="13"/>
-      <c r="AK116" s="13"/>
-      <c r="AL116" s="13"/>
-      <c r="AM116" s="13"/>
-      <c r="AN116" s="13"/>
-      <c r="AO116" s="13"/>
-      <c r="AP116" s="13"/>
-      <c r="AQ116" s="13"/>
-      <c r="AR116" s="13"/>
-      <c r="AS116" s="13"/>
-      <c r="AT116" s="13"/>
-      <c r="AU116" s="13"/>
-      <c r="AV116" s="13"/>
-      <c r="AW116" s="13"/>
-      <c r="AX116" s="13"/>
-      <c r="AY116" s="13"/>
-      <c r="AZ116" s="13"/>
-      <c r="BA116" s="13"/>
-      <c r="BB116" s="13"/>
-      <c r="BC116" s="13"/>
-      <c r="BD116" s="13"/>
-      <c r="BE116" s="13"/>
-      <c r="BF116" s="13"/>
-      <c r="BG116" s="13"/>
-      <c r="BH116" s="13"/>
-      <c r="BI116" s="13"/>
-      <c r="BJ116" s="13"/>
-      <c r="BK116" s="13"/>
-      <c r="BL116" s="13"/>
-      <c r="BM116" s="13"/>
-      <c r="BN116" s="13"/>
-      <c r="BO116" s="13"/>
-      <c r="BP116" s="13"/>
-      <c r="BQ116" s="13"/>
-      <c r="BR116" s="13"/>
-      <c r="BS116" s="13"/>
-      <c r="BT116" s="13"/>
-      <c r="BU116" s="13"/>
-      <c r="BV116" s="13"/>
-      <c r="BW116" s="13"/>
-      <c r="BX116" s="13"/>
-      <c r="BY116" s="13"/>
-      <c r="BZ116" s="13"/>
-      <c r="CA116" s="13"/>
-      <c r="CB116" s="13"/>
-      <c r="CC116" s="13"/>
-      <c r="CD116" s="13"/>
-      <c r="CE116" s="13"/>
-      <c r="CF116" s="13"/>
-      <c r="CG116" s="13"/>
-      <c r="CH116" s="13"/>
-      <c r="CI116" s="13"/>
-      <c r="CJ116" s="13"/>
-      <c r="CK116" s="13"/>
-      <c r="CL116" s="13"/>
-      <c r="CM116" s="13"/>
-      <c r="CN116" s="13"/>
-      <c r="CO116" s="13"/>
-      <c r="CP116" s="13"/>
-      <c r="CQ116" s="13"/>
-      <c r="CR116" s="13"/>
-      <c r="CS116" s="13"/>
-      <c r="CT116" s="13"/>
-      <c r="CU116" s="13"/>
-      <c r="CV116" s="13"/>
-      <c r="CW116" s="13"/>
-      <c r="CX116" s="13"/>
-      <c r="CY116" s="13"/>
-      <c r="CZ116" s="13"/>
-      <c r="DA116" s="13"/>
-      <c r="DB116" s="13"/>
-      <c r="DC116" s="13"/>
-      <c r="DD116" s="13"/>
-      <c r="DE116" s="13"/>
-      <c r="DF116" s="13"/>
-      <c r="DG116" s="13"/>
-      <c r="DH116" s="13"/>
-      <c r="DI116" s="13"/>
-      <c r="DJ116" s="13"/>
-      <c r="DK116" s="13"/>
-      <c r="DL116" s="13"/>
-      <c r="DM116" s="13"/>
-      <c r="DN116" s="13"/>
-      <c r="DO116" s="13"/>
-      <c r="DP116" s="13"/>
-      <c r="DQ116" s="13"/>
-      <c r="DR116" s="13"/>
-      <c r="DS116" s="13"/>
-      <c r="DT116" s="13"/>
-      <c r="DU116" s="13"/>
-      <c r="DV116" s="13"/>
-      <c r="DW116" s="13"/>
-      <c r="DX116" s="13"/>
-      <c r="DY116" s="13"/>
-      <c r="DZ116" s="13"/>
-      <c r="EA116" s="13"/>
-      <c r="EB116" s="13"/>
-      <c r="EC116" s="13"/>
+    <row r="116" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="25"/>
+      <c r="D116" s="10"/>
+      <c r="E116" s="21"/>
+      <c r="F116" s="10"/>
+      <c r="G116" s="10"/>
+      <c r="H116" s="10"/>
+      <c r="I116" s="10"/>
+      <c r="J116" s="10"/>
+      <c r="K116" s="28"/>
+      <c r="L116" s="10"/>
+      <c r="M116" s="10"/>
+      <c r="N116" s="11"/>
+      <c r="O116" s="10"/>
+      <c r="P116" s="21"/>
+      <c r="Q116" s="10"/>
+      <c r="R116" s="28"/>
+      <c r="S116" s="10"/>
+      <c r="T116" s="10"/>
+      <c r="U116" s="10"/>
+      <c r="V116" s="10"/>
+      <c r="W116" s="10"/>
+      <c r="X116" s="10"/>
+      <c r="Y116" s="10"/>
+      <c r="Z116" s="10"/>
+      <c r="AA116" s="21"/>
+      <c r="AB116" s="10"/>
+      <c r="AC116" s="10"/>
+      <c r="AD116" s="10"/>
+      <c r="AE116" s="10"/>
+      <c r="AF116" s="10"/>
+      <c r="AG116" s="10"/>
+      <c r="AH116" s="10"/>
+      <c r="AI116" s="10"/>
+      <c r="AJ116" s="10"/>
+      <c r="AK116" s="10"/>
+      <c r="AL116" s="10"/>
+      <c r="AM116" s="10"/>
+      <c r="AN116" s="27"/>
+      <c r="AO116" s="10"/>
+      <c r="AP116" s="10"/>
+      <c r="AQ116" s="21"/>
+      <c r="AR116" s="10"/>
+      <c r="AS116" s="10"/>
+      <c r="AT116" s="10"/>
+      <c r="AU116" s="28"/>
+      <c r="AV116" s="10"/>
+      <c r="AW116" s="10"/>
+      <c r="AX116" s="10"/>
+      <c r="AY116" s="21"/>
+      <c r="AZ116" s="10"/>
+      <c r="BA116" s="10"/>
+      <c r="BB116" s="10"/>
+      <c r="BC116" s="10"/>
+      <c r="BD116" s="21"/>
+      <c r="BE116" s="10"/>
+      <c r="BF116" s="10"/>
+      <c r="BG116" s="10"/>
+      <c r="BH116" s="10"/>
+      <c r="BI116" s="10"/>
+      <c r="BJ116" s="10"/>
+      <c r="BK116" s="10"/>
+      <c r="BL116" s="10"/>
+      <c r="BM116" s="10"/>
+      <c r="BN116" s="28"/>
+      <c r="BO116" s="10"/>
+      <c r="BP116" s="10"/>
+      <c r="BQ116" s="10"/>
+      <c r="BR116" s="10"/>
+      <c r="BS116" s="10"/>
+      <c r="BT116" s="10"/>
+      <c r="BU116" s="10"/>
+      <c r="BV116" s="10"/>
+      <c r="BW116" s="27"/>
+      <c r="BX116" s="10"/>
+      <c r="BY116" s="28"/>
+      <c r="BZ116" s="10"/>
+      <c r="CA116" s="10"/>
+      <c r="CB116" s="10"/>
     </row>
-    <row r="117" spans="1:133" ht="72" customHeight="1">
+    <row r="117" spans="1:133" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="25"/>
       <c r="D117" s="10"/>
       <c r="E117" s="21"/>
@@ -18129,7 +18105,7 @@
       <c r="CA117" s="10"/>
       <c r="CB117" s="10"/>
     </row>
-    <row r="118" spans="1:133" ht="72" customHeight="1">
+    <row r="118" spans="1:133" x14ac:dyDescent="0.25">
       <c r="B118" s="25"/>
       <c r="D118" s="10"/>
       <c r="E118" s="21"/>
@@ -18209,7 +18185,7 @@
       <c r="CA118" s="10"/>
       <c r="CB118" s="10"/>
     </row>
-    <row r="119" spans="1:133">
+    <row r="119" spans="1:133" x14ac:dyDescent="0.25">
       <c r="B119" s="25"/>
       <c r="D119" s="10"/>
       <c r="E119" s="21"/>
@@ -18289,7 +18265,7 @@
       <c r="CA119" s="10"/>
       <c r="CB119" s="10"/>
     </row>
-    <row r="120" spans="1:133">
+    <row r="120" spans="1:133" x14ac:dyDescent="0.25">
       <c r="B120" s="25"/>
       <c r="D120" s="10"/>
       <c r="E120" s="21"/>
@@ -18369,7 +18345,7 @@
       <c r="CA120" s="10"/>
       <c r="CB120" s="10"/>
     </row>
-    <row r="121" spans="1:133">
+    <row r="121" spans="1:133" x14ac:dyDescent="0.25">
       <c r="B121" s="25"/>
       <c r="D121" s="10"/>
       <c r="E121" s="21"/>
@@ -18449,7 +18425,7 @@
       <c r="CA121" s="10"/>
       <c r="CB121" s="10"/>
     </row>
-    <row r="122" spans="1:133">
+    <row r="122" spans="1:133" x14ac:dyDescent="0.25">
       <c r="B122" s="25"/>
       <c r="D122" s="10"/>
       <c r="E122" s="21"/>
@@ -18529,7 +18505,7 @@
       <c r="CA122" s="10"/>
       <c r="CB122" s="10"/>
     </row>
-    <row r="123" spans="1:133">
+    <row r="123" spans="1:133" x14ac:dyDescent="0.25">
       <c r="B123" s="25"/>
       <c r="D123" s="10"/>
       <c r="E123" s="21"/>
@@ -18609,7 +18585,7 @@
       <c r="CA123" s="10"/>
       <c r="CB123" s="10"/>
     </row>
-    <row r="124" spans="1:133">
+    <row r="124" spans="1:133" x14ac:dyDescent="0.25">
       <c r="B124" s="25"/>
       <c r="D124" s="10"/>
       <c r="E124" s="21"/>
@@ -18689,7 +18665,7 @@
       <c r="CA124" s="10"/>
       <c r="CB124" s="10"/>
     </row>
-    <row r="125" spans="1:133">
+    <row r="125" spans="1:133" x14ac:dyDescent="0.25">
       <c r="B125" s="25"/>
       <c r="D125" s="10"/>
       <c r="E125" s="21"/>
@@ -18769,7 +18745,7 @@
       <c r="CA125" s="10"/>
       <c r="CB125" s="10"/>
     </row>
-    <row r="126" spans="1:133">
+    <row r="126" spans="1:133" x14ac:dyDescent="0.25">
       <c r="B126" s="25"/>
       <c r="D126" s="10"/>
       <c r="E126" s="21"/>
@@ -18849,7 +18825,7 @@
       <c r="CA126" s="10"/>
       <c r="CB126" s="10"/>
     </row>
-    <row r="127" spans="1:133">
+    <row r="127" spans="1:133" x14ac:dyDescent="0.25">
       <c r="B127" s="25"/>
       <c r="D127" s="10"/>
       <c r="E127" s="21"/>
@@ -18929,7 +18905,7 @@
       <c r="CA127" s="10"/>
       <c r="CB127" s="10"/>
     </row>
-    <row r="128" spans="1:133">
+    <row r="128" spans="1:133" x14ac:dyDescent="0.25">
       <c r="B128" s="25"/>
       <c r="D128" s="10"/>
       <c r="E128" s="21"/>
@@ -19009,7 +18985,7 @@
       <c r="CA128" s="10"/>
       <c r="CB128" s="10"/>
     </row>
-    <row r="129" spans="2:80">
+    <row r="129" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B129" s="25"/>
       <c r="D129" s="10"/>
       <c r="E129" s="21"/>
@@ -19089,7 +19065,7 @@
       <c r="CA129" s="10"/>
       <c r="CB129" s="10"/>
     </row>
-    <row r="130" spans="2:80">
+    <row r="130" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B130" s="25"/>
       <c r="D130" s="10"/>
       <c r="E130" s="21"/>
@@ -19169,7 +19145,7 @@
       <c r="CA130" s="10"/>
       <c r="CB130" s="10"/>
     </row>
-    <row r="131" spans="2:80">
+    <row r="131" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B131" s="25"/>
       <c r="D131" s="10"/>
       <c r="E131" s="21"/>
@@ -19249,7 +19225,7 @@
       <c r="CA131" s="10"/>
       <c r="CB131" s="10"/>
     </row>
-    <row r="132" spans="2:80">
+    <row r="132" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B132" s="25"/>
       <c r="D132" s="10"/>
       <c r="E132" s="21"/>
@@ -19329,7 +19305,7 @@
       <c r="CA132" s="10"/>
       <c r="CB132" s="10"/>
     </row>
-    <row r="133" spans="2:80">
+    <row r="133" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B133" s="25"/>
       <c r="D133" s="10"/>
       <c r="E133" s="21"/>
@@ -19409,7 +19385,7 @@
       <c r="CA133" s="10"/>
       <c r="CB133" s="10"/>
     </row>
-    <row r="134" spans="2:80">
+    <row r="134" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B134" s="25"/>
       <c r="D134" s="10"/>
       <c r="E134" s="21"/>
@@ -19489,7 +19465,7 @@
       <c r="CA134" s="10"/>
       <c r="CB134" s="10"/>
     </row>
-    <row r="135" spans="2:80">
+    <row r="135" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B135" s="25"/>
       <c r="D135" s="10"/>
       <c r="E135" s="21"/>
@@ -19569,7 +19545,7 @@
       <c r="CA135" s="10"/>
       <c r="CB135" s="10"/>
     </row>
-    <row r="136" spans="2:80">
+    <row r="136" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B136" s="25"/>
       <c r="D136" s="10"/>
       <c r="E136" s="21"/>
@@ -19649,7 +19625,7 @@
       <c r="CA136" s="10"/>
       <c r="CB136" s="10"/>
     </row>
-    <row r="137" spans="2:80">
+    <row r="137" spans="2:80" x14ac:dyDescent="0.25">
       <c r="B137" s="25"/>
       <c r="D137" s="10"/>
       <c r="E137" s="21"/>
@@ -19729,8 +19705,7 @@
       <c r="CA137" s="10"/>
       <c r="CB137" s="10"/>
     </row>
-    <row r="138" spans="2:80">
-      <c r="B138" s="25"/>
+    <row r="138" spans="2:80" x14ac:dyDescent="0.25">
       <c r="D138" s="10"/>
       <c r="E138" s="21"/>
       <c r="F138" s="10"/>
@@ -19809,7 +19784,7 @@
       <c r="CA138" s="10"/>
       <c r="CB138" s="10"/>
     </row>
-    <row r="139" spans="2:80">
+    <row r="139" spans="2:80" x14ac:dyDescent="0.25">
       <c r="D139" s="10"/>
       <c r="E139" s="21"/>
       <c r="F139" s="10"/>
@@ -19888,7 +19863,7 @@
       <c r="CA139" s="10"/>
       <c r="CB139" s="10"/>
     </row>
-    <row r="140" spans="2:80">
+    <row r="140" spans="2:80" x14ac:dyDescent="0.25">
       <c r="D140" s="10"/>
       <c r="E140" s="21"/>
       <c r="F140" s="10"/>
@@ -19967,7 +19942,7 @@
       <c r="CA140" s="10"/>
       <c r="CB140" s="10"/>
     </row>
-    <row r="141" spans="2:80">
+    <row r="141" spans="2:80" x14ac:dyDescent="0.25">
       <c r="D141" s="10"/>
       <c r="E141" s="21"/>
       <c r="F141" s="10"/>
@@ -20046,7 +20021,7 @@
       <c r="CA141" s="10"/>
       <c r="CB141" s="10"/>
     </row>
-    <row r="142" spans="2:80">
+    <row r="142" spans="2:80" x14ac:dyDescent="0.25">
       <c r="D142" s="10"/>
       <c r="E142" s="21"/>
       <c r="F142" s="10"/>
@@ -20125,7 +20100,7 @@
       <c r="CA142" s="10"/>
       <c r="CB142" s="10"/>
     </row>
-    <row r="143" spans="2:80">
+    <row r="143" spans="2:80" x14ac:dyDescent="0.25">
       <c r="D143" s="10"/>
       <c r="E143" s="21"/>
       <c r="F143" s="10"/>
@@ -20204,7 +20179,7 @@
       <c r="CA143" s="10"/>
       <c r="CB143" s="10"/>
     </row>
-    <row r="144" spans="2:80">
+    <row r="144" spans="2:80" x14ac:dyDescent="0.25">
       <c r="D144" s="10"/>
       <c r="E144" s="21"/>
       <c r="F144" s="10"/>
@@ -20283,7 +20258,7 @@
       <c r="CA144" s="10"/>
       <c r="CB144" s="10"/>
     </row>
-    <row r="145" spans="4:80">
+    <row r="145" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D145" s="10"/>
       <c r="E145" s="21"/>
       <c r="F145" s="10"/>
@@ -20362,7 +20337,7 @@
       <c r="CA145" s="10"/>
       <c r="CB145" s="10"/>
     </row>
-    <row r="146" spans="4:80">
+    <row r="146" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D146" s="10"/>
       <c r="E146" s="21"/>
       <c r="F146" s="10"/>
@@ -20441,7 +20416,7 @@
       <c r="CA146" s="10"/>
       <c r="CB146" s="10"/>
     </row>
-    <row r="147" spans="4:80">
+    <row r="147" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D147" s="10"/>
       <c r="E147" s="21"/>
       <c r="F147" s="10"/>
@@ -20520,7 +20495,7 @@
       <c r="CA147" s="10"/>
       <c r="CB147" s="10"/>
     </row>
-    <row r="148" spans="4:80">
+    <row r="148" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D148" s="10"/>
       <c r="E148" s="21"/>
       <c r="F148" s="10"/>
@@ -20599,7 +20574,7 @@
       <c r="CA148" s="10"/>
       <c r="CB148" s="10"/>
     </row>
-    <row r="149" spans="4:80">
+    <row r="149" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D149" s="10"/>
       <c r="E149" s="21"/>
       <c r="F149" s="10"/>
@@ -20678,7 +20653,7 @@
       <c r="CA149" s="10"/>
       <c r="CB149" s="10"/>
     </row>
-    <row r="150" spans="4:80">
+    <row r="150" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D150" s="10"/>
       <c r="E150" s="21"/>
       <c r="F150" s="10"/>
@@ -20757,7 +20732,7 @@
       <c r="CA150" s="10"/>
       <c r="CB150" s="10"/>
     </row>
-    <row r="151" spans="4:80">
+    <row r="151" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D151" s="10"/>
       <c r="E151" s="21"/>
       <c r="F151" s="10"/>
@@ -20836,7 +20811,7 @@
       <c r="CA151" s="10"/>
       <c r="CB151" s="10"/>
     </row>
-    <row r="152" spans="4:80">
+    <row r="152" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D152" s="10"/>
       <c r="E152" s="21"/>
       <c r="F152" s="10"/>
@@ -20915,7 +20890,7 @@
       <c r="CA152" s="10"/>
       <c r="CB152" s="10"/>
     </row>
-    <row r="153" spans="4:80">
+    <row r="153" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D153" s="10"/>
       <c r="E153" s="21"/>
       <c r="F153" s="10"/>
@@ -20994,7 +20969,7 @@
       <c r="CA153" s="10"/>
       <c r="CB153" s="10"/>
     </row>
-    <row r="154" spans="4:80">
+    <row r="154" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D154" s="10"/>
       <c r="E154" s="21"/>
       <c r="F154" s="10"/>
@@ -21073,7 +21048,7 @@
       <c r="CA154" s="10"/>
       <c r="CB154" s="10"/>
     </row>
-    <row r="155" spans="4:80">
+    <row r="155" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D155" s="10"/>
       <c r="E155" s="21"/>
       <c r="F155" s="10"/>
@@ -21152,7 +21127,7 @@
       <c r="CA155" s="10"/>
       <c r="CB155" s="10"/>
     </row>
-    <row r="156" spans="4:80">
+    <row r="156" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D156" s="10"/>
       <c r="E156" s="21"/>
       <c r="F156" s="10"/>
@@ -21231,7 +21206,7 @@
       <c r="CA156" s="10"/>
       <c r="CB156" s="10"/>
     </row>
-    <row r="157" spans="4:80">
+    <row r="157" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D157" s="10"/>
       <c r="E157" s="21"/>
       <c r="F157" s="10"/>
@@ -21310,7 +21285,7 @@
       <c r="CA157" s="10"/>
       <c r="CB157" s="10"/>
     </row>
-    <row r="158" spans="4:80">
+    <row r="158" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D158" s="10"/>
       <c r="E158" s="21"/>
       <c r="F158" s="10"/>
@@ -21389,7 +21364,7 @@
       <c r="CA158" s="10"/>
       <c r="CB158" s="10"/>
     </row>
-    <row r="159" spans="4:80">
+    <row r="159" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D159" s="10"/>
       <c r="E159" s="21"/>
       <c r="F159" s="10"/>
@@ -21468,7 +21443,7 @@
       <c r="CA159" s="10"/>
       <c r="CB159" s="10"/>
     </row>
-    <row r="160" spans="4:80">
+    <row r="160" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D160" s="10"/>
       <c r="E160" s="21"/>
       <c r="F160" s="10"/>
@@ -21547,7 +21522,7 @@
       <c r="CA160" s="10"/>
       <c r="CB160" s="10"/>
     </row>
-    <row r="161" spans="4:80">
+    <row r="161" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D161" s="10"/>
       <c r="E161" s="21"/>
       <c r="F161" s="10"/>
@@ -21626,7 +21601,7 @@
       <c r="CA161" s="10"/>
       <c r="CB161" s="10"/>
     </row>
-    <row r="162" spans="4:80">
+    <row r="162" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D162" s="10"/>
       <c r="E162" s="21"/>
       <c r="F162" s="10"/>
@@ -21705,7 +21680,7 @@
       <c r="CA162" s="10"/>
       <c r="CB162" s="10"/>
     </row>
-    <row r="163" spans="4:80">
+    <row r="163" spans="4:80" x14ac:dyDescent="0.25">
       <c r="D163" s="10"/>
       <c r="E163" s="21"/>
       <c r="F163" s="10"/>
@@ -21784,85 +21759,6 @@
       <c r="CA163" s="10"/>
       <c r="CB163" s="10"/>
     </row>
-    <row r="164" spans="4:80">
-      <c r="D164" s="10"/>
-      <c r="E164" s="21"/>
-      <c r="F164" s="10"/>
-      <c r="G164" s="10"/>
-      <c r="H164" s="10"/>
-      <c r="I164" s="10"/>
-      <c r="J164" s="10"/>
-      <c r="K164" s="28"/>
-      <c r="L164" s="10"/>
-      <c r="M164" s="10"/>
-      <c r="N164" s="11"/>
-      <c r="O164" s="10"/>
-      <c r="P164" s="21"/>
-      <c r="Q164" s="10"/>
-      <c r="R164" s="28"/>
-      <c r="S164" s="10"/>
-      <c r="T164" s="10"/>
-      <c r="U164" s="10"/>
-      <c r="V164" s="10"/>
-      <c r="W164" s="10"/>
-      <c r="X164" s="10"/>
-      <c r="Y164" s="10"/>
-      <c r="Z164" s="10"/>
-      <c r="AA164" s="21"/>
-      <c r="AB164" s="10"/>
-      <c r="AC164" s="10"/>
-      <c r="AD164" s="10"/>
-      <c r="AE164" s="10"/>
-      <c r="AF164" s="10"/>
-      <c r="AG164" s="10"/>
-      <c r="AH164" s="10"/>
-      <c r="AI164" s="10"/>
-      <c r="AJ164" s="10"/>
-      <c r="AK164" s="10"/>
-      <c r="AL164" s="10"/>
-      <c r="AM164" s="10"/>
-      <c r="AN164" s="27"/>
-      <c r="AO164" s="10"/>
-      <c r="AP164" s="10"/>
-      <c r="AQ164" s="21"/>
-      <c r="AR164" s="10"/>
-      <c r="AS164" s="10"/>
-      <c r="AT164" s="10"/>
-      <c r="AU164" s="28"/>
-      <c r="AV164" s="10"/>
-      <c r="AW164" s="10"/>
-      <c r="AX164" s="10"/>
-      <c r="AY164" s="21"/>
-      <c r="AZ164" s="10"/>
-      <c r="BA164" s="10"/>
-      <c r="BB164" s="10"/>
-      <c r="BC164" s="10"/>
-      <c r="BD164" s="21"/>
-      <c r="BE164" s="10"/>
-      <c r="BF164" s="10"/>
-      <c r="BG164" s="10"/>
-      <c r="BH164" s="10"/>
-      <c r="BI164" s="10"/>
-      <c r="BJ164" s="10"/>
-      <c r="BK164" s="10"/>
-      <c r="BL164" s="10"/>
-      <c r="BM164" s="10"/>
-      <c r="BN164" s="28"/>
-      <c r="BO164" s="10"/>
-      <c r="BP164" s="10"/>
-      <c r="BQ164" s="10"/>
-      <c r="BR164" s="10"/>
-      <c r="BS164" s="10"/>
-      <c r="BT164" s="10"/>
-      <c r="BU164" s="10"/>
-      <c r="BV164" s="10"/>
-      <c r="BW164" s="27"/>
-      <c r="BX164" s="10"/>
-      <c r="BY164" s="28"/>
-      <c r="BZ164" s="10"/>
-      <c r="CA164" s="10"/>
-      <c r="CB164" s="10"/>
-    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A2:B3"/>
@@ -21875,7 +21771,7 @@
     <hyperlink ref="A37" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updating the Fun_with_HBase template
</commit_message>
<xml_diff>
--- a/NiFi Templates.xlsx
+++ b/NiFi Templates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-102400" yWindow="-15400" windowWidth="36540" windowHeight="20440" tabRatio="500"/>
+    <workbookView xWindow="-51200" yWindow="-10820" windowWidth="51200" windowHeight="28340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="218">
   <si>
     <t>Template Name:</t>
   </si>
@@ -685,6 +685,9 @@
   </si>
   <si>
     <t>PutElasticsearch</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1466,10 +1469,10 @@
   <dimension ref="A1:ED164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="CL47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="D28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="EA47" sqref="EA47"/>
+      <selection pane="bottomRight" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1767,6 +1770,10 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="BW1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="BX1">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1797,7 +1804,7 @@
       </c>
       <c r="CE1">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="CF1">
         <f t="shared" si="1"/>
@@ -1865,7 +1872,7 @@
       </c>
       <c r="CW1">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CX1">
         <f t="shared" si="2"/>
@@ -1921,7 +1928,7 @@
       </c>
       <c r="DL1">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="DM1">
         <f t="shared" si="2"/>
@@ -5735,7 +5742,9 @@
       <c r="F28" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="G28" s="13"/>
+      <c r="G28" s="13" t="s">
+        <v>182</v>
+      </c>
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
       <c r="J28" s="13" t="s">
@@ -5821,7 +5830,9 @@
       <c r="CB28" s="13"/>
       <c r="CC28" s="13"/>
       <c r="CD28" s="13"/>
-      <c r="CE28" s="13"/>
+      <c r="CE28" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="CF28" s="13"/>
       <c r="CG28" s="13"/>
       <c r="CH28" s="13"/>
@@ -5843,11 +5854,11 @@
       </c>
       <c r="CU28" s="13"/>
       <c r="CV28" s="13"/>
-      <c r="CW28" s="13" t="s">
-        <v>27</v>
-      </c>
+      <c r="CW28" s="13"/>
       <c r="CX28" s="13"/>
-      <c r="CY28" s="13"/>
+      <c r="CY28" s="13" t="s">
+        <v>217</v>
+      </c>
       <c r="CZ28" s="13"/>
       <c r="DA28" s="13"/>
       <c r="DB28" s="13"/>
@@ -5860,7 +5871,9 @@
       <c r="DI28" s="13"/>
       <c r="DJ28" s="13"/>
       <c r="DK28" s="13"/>
-      <c r="DL28" s="13"/>
+      <c r="DL28" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="DM28" s="13"/>
       <c r="DN28" s="13"/>
       <c r="DO28" s="13"/>

</xml_diff>

<commit_message>
updated XLS file and flow layout
</commit_message>
<xml_diff>
--- a/NiFi Templates.xlsx
+++ b/NiFi Templates.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="219">
   <si>
     <t>Template Name:</t>
   </si>
@@ -1480,10 +1480,10 @@
   <dimension ref="A1:ED164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="CM9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="CK45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="EA48" sqref="EA48"/>
+      <selection pane="bottomRight" activeCell="DH48" sqref="DH48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1615,11 +1615,11 @@
       </c>
       <c r="AG1">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AH1">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AI1">
         <f t="shared" si="1"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="DH1">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="DI1">
         <f t="shared" si="2"/>
@@ -8857,10 +8857,10 @@
       <c r="AD48" s="13"/>
       <c r="AE48" s="13"/>
       <c r="AF48" s="13"/>
-      <c r="AG48" s="13"/>
-      <c r="AH48" s="13" t="s">
+      <c r="AG48" s="13" t="s">
         <v>191</v>
       </c>
+      <c r="AH48" s="13"/>
       <c r="AI48" s="13"/>
       <c r="AJ48" s="13"/>
       <c r="AK48" s="13"/>
@@ -8946,7 +8946,9 @@
       <c r="DE48" s="13"/>
       <c r="DF48" s="13"/>
       <c r="DG48" s="13"/>
-      <c r="DH48" s="13"/>
+      <c r="DH48" s="13" t="s">
+        <v>191</v>
+      </c>
       <c r="DI48" s="13"/>
       <c r="DJ48" s="13"/>
       <c r="DK48" s="13"/>

</xml_diff>

<commit_message>
Added ConvertCSVtoCQL (Cassandra) template
</commit_message>
<xml_diff>
--- a/NiFi Templates.xlsx
+++ b/NiFi Templates.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-10820" windowWidth="51200" windowHeight="28340" tabRatio="500"/>
+    <workbookView xWindow="6340" yWindow="1140" windowWidth="39940" windowHeight="24340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="220">
   <si>
     <t>Template Name:</t>
   </si>
@@ -688,6 +688,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ConvertCSVtoCQL</t>
+  </si>
+  <si>
+    <t>Describes a flow where a CSV file (whose filename and content) contributes to the fields in a Cassandra table is processed, then CQL statements are constructed and executed.</t>
   </si>
 </sst>
 </file>
@@ -1469,10 +1475,10 @@
   <dimension ref="A1:ED164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="D28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="D41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="G28" sqref="G28"/>
+      <selection pane="bottomRight" activeCell="EA49" sqref="EA49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1636,7 +1642,7 @@
       </c>
       <c r="AO1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP1">
         <f t="shared" si="1"/>
@@ -1656,7 +1662,7 @@
       </c>
       <c r="AT1">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AU1">
         <f t="shared" si="1"/>
@@ -1772,7 +1778,7 @@
       </c>
       <c r="BW1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX1">
         <f t="shared" si="1"/>
@@ -1912,7 +1918,7 @@
       </c>
       <c r="DH1">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="DI1">
         <f t="shared" si="2"/>
@@ -1964,7 +1970,7 @@
       </c>
       <c r="DU1">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="DV1">
         <f t="shared" si="2"/>
@@ -1988,7 +1994,7 @@
       </c>
       <c r="EA1">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="EB1">
         <f t="shared" si="2"/>
@@ -8817,8 +8823,12 @@
       <c r="EC47" s="13"/>
     </row>
     <row r="48" spans="1:133" ht="72" customHeight="1">
-      <c r="A48" s="16"/>
-      <c r="B48" s="24"/>
+      <c r="A48" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>219</v>
+      </c>
       <c r="D48" s="18"/>
       <c r="E48" s="18"/>
       <c r="F48" s="13"/>
@@ -8856,12 +8866,16 @@
       <c r="AL48" s="13"/>
       <c r="AM48" s="13"/>
       <c r="AN48" s="13"/>
-      <c r="AO48" s="13"/>
+      <c r="AO48" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="AP48" s="13"/>
       <c r="AQ48" s="13"/>
       <c r="AR48" s="13"/>
       <c r="AS48" s="13"/>
-      <c r="AT48" s="13"/>
+      <c r="AT48" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="AU48" s="13"/>
       <c r="AV48" s="13"/>
       <c r="AW48" s="13"/>
@@ -8890,7 +8904,9 @@
       <c r="BT48" s="13"/>
       <c r="BU48" s="13"/>
       <c r="BV48" s="13"/>
-      <c r="BW48" s="13"/>
+      <c r="BW48" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="BX48" s="13"/>
       <c r="BY48" s="13"/>
       <c r="BZ48" s="13"/>
@@ -8905,7 +8921,9 @@
       <c r="CI48" s="13"/>
       <c r="CJ48" s="13"/>
       <c r="CK48" s="13"/>
-      <c r="CL48" s="13"/>
+      <c r="CL48" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="CM48" s="13"/>
       <c r="CN48" s="13"/>
       <c r="CO48" s="13"/>
@@ -8927,7 +8945,9 @@
       <c r="DE48" s="13"/>
       <c r="DF48" s="13"/>
       <c r="DG48" s="13"/>
-      <c r="DH48" s="13"/>
+      <c r="DH48" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="DI48" s="13"/>
       <c r="DJ48" s="13"/>
       <c r="DK48" s="13"/>
@@ -8940,13 +8960,17 @@
       <c r="DR48" s="13"/>
       <c r="DS48" s="13"/>
       <c r="DT48" s="13"/>
-      <c r="DU48" s="13"/>
+      <c r="DU48" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="DV48" s="13"/>
       <c r="DW48" s="13"/>
       <c r="DX48" s="13"/>
       <c r="DY48" s="13"/>
       <c r="DZ48" s="13"/>
-      <c r="EA48" s="13"/>
+      <c r="EA48" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="EB48" s="13"/>
       <c r="EC48" s="13"/>
     </row>

</xml_diff>